<commit_message>
Cambios del arvhico conjuntos residenciales event storming
</commit_message>
<xml_diff>
--- a/Doo-Doc/Seccion # 7/ConjuntosResidenciales - Event Storming.xlsx
+++ b/Doo-Doc/Seccion # 7/ConjuntosResidenciales - Event Storming.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\DOO 2024 BD\DOO\victus-doc\Doo-Doc\Seccion # 7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uconet-my.sharepoint.com/personal/juan_avendano1956_uco_net_co/Documents/Documents/victus-doc/Doo-Doc/Seccion # 7/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1F0B49-DD34-4DE4-8D57-041CC992534B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="147" documentId="13_ncr:1_{6A1F0B49-DD34-4DE4-8D57-041CC992534B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7914160D-F503-420A-8B7C-6C1ECD514C3B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="7" xr2:uid="{36012E7C-B3F4-482B-AC16-7CCB81B9AE88}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="5" xr2:uid="{36012E7C-B3F4-482B-AC16-7CCB81B9AE88}"/>
   </bookViews>
   <sheets>
     <sheet name="Flujo de eventos en el tiempo" sheetId="61" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="96">
   <si>
     <t>Descripción</t>
   </si>
@@ -175,27 +175,6 @@
     <t>Zona común creada</t>
   </si>
   <si>
-    <t>nombre zona común modificado</t>
-  </si>
-  <si>
-    <t>Imagen zona común modificado</t>
-  </si>
-  <si>
-    <t>Descripción zona común modificado</t>
-  </si>
-  <si>
-    <t>Capacidad zona común modificado</t>
-  </si>
-  <si>
-    <t>hora de apertura zona común modificado</t>
-  </si>
-  <si>
-    <t>Hora de cierre zona común modificado</t>
-  </si>
-  <si>
-    <t>ID conjunto residencial asociado</t>
-  </si>
-  <si>
     <t>Zona común deshabilitada</t>
   </si>
   <si>
@@ -226,21 +205,6 @@
     <t xml:space="preserve">Agenda buscada </t>
   </si>
   <si>
-    <t>nombre agenda modificado</t>
-  </si>
-  <si>
-    <t>Día agenda modificado</t>
-  </si>
-  <si>
-    <t>ID zona común asignado</t>
-  </si>
-  <si>
-    <t>Agenda registrada</t>
-  </si>
-  <si>
-    <t>Turnos Agenda modificados</t>
-  </si>
-  <si>
     <t>Agenda eliminada</t>
   </si>
   <si>
@@ -262,18 +226,6 @@
     <t>Turno creado</t>
   </si>
   <si>
-    <t>Turno buscado</t>
-  </si>
-  <si>
-    <t>número de turno turno modificado</t>
-  </si>
-  <si>
-    <t>Hora de inicio turno modificada</t>
-  </si>
-  <si>
-    <t>Hora de finalización turno modificada</t>
-  </si>
-  <si>
     <t>Turno eliminado</t>
   </si>
   <si>
@@ -299,6 +251,93 @@
   </si>
   <si>
     <t>Gestión de conjuntos residenciales</t>
+  </si>
+  <si>
+    <t>Agenda modificada</t>
+  </si>
+  <si>
+    <t>Acción de buscar la agenda correspondiente a la zona común.</t>
+  </si>
+  <si>
+    <t>Modificar agenda</t>
+  </si>
+  <si>
+    <t>Agenda creada</t>
+  </si>
+  <si>
+    <t>Acción de modificar los datos que contiene la agenda</t>
+  </si>
+  <si>
+    <t>Crear agenda</t>
+  </si>
+  <si>
+    <t>actor</t>
+  </si>
+  <si>
+    <t>Residente</t>
+  </si>
+  <si>
+    <t>Buscar agenda</t>
+  </si>
+  <si>
+    <t>Adminitrador</t>
+  </si>
+  <si>
+    <t>Acción de crear una agenda</t>
+  </si>
+  <si>
+    <t>Elilimar agenda</t>
+  </si>
+  <si>
+    <t>Acción que permite eliminar completamente una agenda</t>
+  </si>
+  <si>
+    <t>Agenda-Pol-0001</t>
+  </si>
+  <si>
+    <t>No pueden haber más de una agenda con la misma zona común</t>
+  </si>
+  <si>
+    <t>La agenda no puede contener turnos que no estén dentro de los horarios de la zona común.</t>
+  </si>
+  <si>
+    <t>Agenda-Pol-0002</t>
+  </si>
+  <si>
+    <t>Agenda-Pol-0003</t>
+  </si>
+  <si>
+    <t>La agenda no puede tener más de una zona común asociada.</t>
+  </si>
+  <si>
+    <t>Turno modificado</t>
+  </si>
+  <si>
+    <t>Turno-Pol-0001</t>
+  </si>
+  <si>
+    <t>No pueden haber más de un turno a la misma hora de inicio y finalización para la misma agenda.</t>
+  </si>
+  <si>
+    <t>Turno-Pol-0002</t>
+  </si>
+  <si>
+    <t>El</t>
+  </si>
+  <si>
+    <t>La agenda necesita de una zona común asociada</t>
+  </si>
+  <si>
+    <t>Conjunto residencial</t>
+  </si>
+  <si>
+    <t>Define a que conjunto residencial pertenece la zona común</t>
+  </si>
+  <si>
+    <t>Información de la zona común</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Información de la zona común </t>
   </si>
 </sst>
 </file>
@@ -468,7 +507,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -753,13 +792,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -822,6 +872,21 @@
     <xf numFmtId="0" fontId="5" fillId="17" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="16" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -831,15 +896,57 @@
     <xf numFmtId="0" fontId="6" fillId="16" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -849,38 +956,11 @@
     <xf numFmtId="0" fontId="4" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -966,35 +1046,56 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1098,6 +1199,46 @@
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Valores"/>
+      <sheetName val="ContextMapping"/>
+      <sheetName val="Contextos"/>
+      <sheetName val=" Gestión de Conjuntos residenci"/>
+      <sheetName val="Gestión de Residentes"/>
+      <sheetName val="Reservas"/>
+      <sheetName val="Reserva-0001"/>
+      <sheetName val="Reserva-0002"/>
+      <sheetName val="Reserva-0003"/>
+      <sheetName val="CaracterizaciónContexto1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="2">
+        <row r="5">
+          <cell r="D5" t="str">
+            <v>Contexto cuya motivación es Gestionar la estructura física y los recursos disponibles en cada conjunto residencial. Aquí se manejan los datos sobre qué conjuntos existen, dónde están ubicados, qué recursos ofrecen según una Agenda con respectivos turnos para cada zona.</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Flujo de eventos en el tiempo"/>
       <sheetName val="Listado Objetos de Dominio"/>
@@ -1138,46 +1279,6 @@
       <sheetData sheetId="5" refreshError="1"/>
       <sheetData sheetId="6" refreshError="1"/>
       <sheetData sheetId="7" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Valores"/>
-      <sheetName val="ContextMapping"/>
-      <sheetName val="Contextos"/>
-      <sheetName val=" Gestión de Conjuntos residenci"/>
-      <sheetName val="Gestión de Residentes"/>
-      <sheetName val="Reservas"/>
-      <sheetName val="Reserva-0001"/>
-      <sheetName val="Reserva-0002"/>
-      <sheetName val="Reserva-0003"/>
-      <sheetName val="CaracterizaciónContexto1"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2">
-        <row r="5">
-          <cell r="D5" t="str">
-            <v>Contexto cuya motivación es Gestionar la estructura física y los recursos disponibles en cada conjunto residencial. Aquí se manejan los datos sobre qué conjuntos existen, dónde están ubicados, qué recursos ofrecen según una Agenda con respectivos turnos para cada zona.</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1484,15 +1585,15 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="11.42578125" style="2"/>
+    <col min="1" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1"/>
     </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F18"/>
     </row>
   </sheetData>
@@ -1508,39 +1609,39 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="2" max="2" width="50.7109375" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5546875" customWidth="1"/>
+    <col min="2" max="2" width="50.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="4" max="4" width="22.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="78" t="s">
-        <v>82</v>
-      </c>
-      <c r="C1" s="78"/>
-      <c r="D1" s="79"/>
-    </row>
-    <row r="2" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="25"/>
+      <c r="D1" s="26"/>
+    </row>
+    <row r="2" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="22" t="str">
-        <f>[2]Contextos!$D$5</f>
+      <c r="B2" s="27" t="str">
+        <f>[1]Contextos!$D$5</f>
         <v>Contexto cuya motivación es Gestionar la estructura física y los recursos disponibles en cada conjunto residencial. Aquí se manejan los datos sobre qué conjuntos existen, dónde están ubicados, qué recursos ofrecen según una Agenda con respectivos turnos para cada zona.</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="24"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C2" s="28"/>
+      <c r="D2" s="29"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>4</v>
       </c>
@@ -1554,80 +1655,80 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="72" t="s">
+    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="73" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4" s="74" t="s">
+      <c r="B4" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="75" t="str">
+      <c r="D4" s="30" t="str">
         <f>$B$1</f>
         <v>Gestión de conjuntos residenciales</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="72" t="s">
+    <row r="5" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="73" t="s">
-        <v>76</v>
-      </c>
-      <c r="C5" s="74" t="s">
+      <c r="B5" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="76"/>
-    </row>
-    <row r="6" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="72" t="s">
+      <c r="D5" s="31"/>
+    </row>
+    <row r="6" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="73" t="s">
-        <v>77</v>
-      </c>
-      <c r="C6" s="74" t="s">
+      <c r="B6" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="76"/>
-    </row>
-    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="72" t="s">
+      <c r="D6" s="31"/>
+    </row>
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="73" t="s">
-        <v>78</v>
-      </c>
-      <c r="C7" s="74" t="s">
+      <c r="B7" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="76"/>
-    </row>
-    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="72" t="s">
+      <c r="D7" s="31"/>
+    </row>
+    <row r="8" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="73" t="s">
-        <v>79</v>
-      </c>
-      <c r="C8" s="74" t="s">
+      <c r="B8" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="76"/>
-    </row>
-    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="72" t="s">
-        <v>80</v>
-      </c>
-      <c r="B9" s="73" t="s">
-        <v>81</v>
-      </c>
-      <c r="C9" s="74" t="s">
+      <c r="D8" s="31"/>
+    </row>
+    <row r="9" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9" s="22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="77"/>
+      <c r="D9" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1656,108 +1757,108 @@
       <selection sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="18.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="28.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="18.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="28.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="38" style="1" customWidth="1"/>
-    <col min="13" max="13" width="46.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="132.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="50.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="66.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="52.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.42578125" style="1"/>
+    <col min="13" max="13" width="46.33203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="132.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="50.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="66.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="52.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="40" t="str">
-        <f>'[1]Listado Objetos de Dominio'!A4</f>
+      <c r="B2" s="43" t="str">
+        <f>'[2]Listado Objetos de Dominio'!A4</f>
         <v>ConjuntoResidencial</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="41"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="44"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="25" t="str">
+      <c r="B3" s="45" t="str">
         <f>'Listado Objetos de Dominio'!$B$5</f>
         <v>Objeto de dominio que representa a cada una de las zonas comunes que se encuentran dentro de un conjunto residencial para que los residentes puedan reservar esos espacios y porder usarlos.</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="26"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="45"/>
+      <c r="M3" s="46"/>
       <c r="N3" s="4"/>
     </row>
-    <row r="4" spans="1:14" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="29.1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="27"/>
+      <c r="C4" s="35"/>
       <c r="D4" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="28"/>
-      <c r="G4" s="35" t="s">
+      <c r="F4" s="47"/>
+      <c r="G4" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="35"/>
+      <c r="H4" s="38"/>
       <c r="I4" s="9" t="s">
         <v>14</v>
       </c>
@@ -1767,52 +1868,52 @@
       <c r="K4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="38" t="s">
+      <c r="L4" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="39" t="s">
+      <c r="M4" s="42" t="s">
         <v>18</v>
       </c>
       <c r="N4" s="4"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="28"/>
-      <c r="G5" s="33" t="s">
+      <c r="F5" s="47"/>
+      <c r="G5" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="33"/>
-      <c r="I5" s="36" t="s">
+      <c r="H5" s="36"/>
+      <c r="I5" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="37" t="s">
+      <c r="J5" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="34" t="s">
+      <c r="K5" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="38"/>
-      <c r="M5" s="39"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="30"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="42"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="34"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="49"/>
       <c r="E6" s="14" t="s">
         <v>21</v>
       </c>
@@ -1825,13 +1926,13 @@
       <c r="H6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="36"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="39"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I6" s="39"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="42"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="11"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
@@ -1848,7 +1949,7 @@
       <c r="L7" s="12"/>
       <c r="M7" s="13"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="11"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -1865,7 +1966,7 @@
       <c r="L8" s="12"/>
       <c r="M8" s="13"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="11"/>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
@@ -1882,7 +1983,7 @@
       <c r="L9" s="12"/>
       <c r="M9" s="13"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="11"/>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
@@ -1899,7 +2000,7 @@
       <c r="L10" s="12"/>
       <c r="M10" s="13"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="11"/>
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
@@ -1916,7 +2017,7 @@
       <c r="L11" s="12"/>
       <c r="M11" s="13"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
@@ -1935,6 +2036,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="D5:D6"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:B6"/>
@@ -1951,7 +2053,6 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="E5:F5"/>
-    <mergeCell ref="D5:D6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{55E21CA2-8FF8-4D5B-80A8-5761C952FB5A}"/>
@@ -1965,115 +2066,115 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9732BFC6-5B3A-4E40-BEA3-58E7EDB79B0C}">
-  <dimension ref="A1:N16"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:N1"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="18.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="37.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="18.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="37.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="38" style="1" customWidth="1"/>
-    <col min="13" max="13" width="46.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="132.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="50.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="66.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="52.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.42578125" style="1"/>
+    <col min="13" max="13" width="46.33203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="132.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="50.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="66.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="52.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="44" t="str">
-        <f>'[1]Listado Objetos de Dominio'!A5</f>
+      <c r="B2" s="54" t="str">
+        <f>'[2]Listado Objetos de Dominio'!A5</f>
         <v>ZonaComun</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="46"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="56"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="47" t="str">
+      <c r="B3" s="57" t="str">
         <f>'Listado Objetos de Dominio'!$B$5</f>
         <v>Objeto de dominio que representa a cada una de las zonas comunes que se encuentran dentro de un conjunto residencial para que los residentes puedan reservar esos espacios y porder usarlos.</v>
       </c>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="48"/>
-      <c r="M3" s="49"/>
+      <c r="C3" s="58"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="59"/>
       <c r="N3" s="4"/>
     </row>
-    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="51"/>
+      <c r="C4" s="61"/>
       <c r="D4" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="52" t="s">
+      <c r="E4" s="62" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="53"/>
-      <c r="G4" s="54" t="s">
+      <c r="F4" s="63"/>
+      <c r="G4" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="55"/>
+      <c r="H4" s="65"/>
       <c r="I4" s="9" t="s">
         <v>14</v>
       </c>
@@ -2083,52 +2184,52 @@
       <c r="K4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="56" t="s">
+      <c r="L4" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="59" t="s">
+      <c r="M4" s="69" t="s">
         <v>18</v>
       </c>
       <c r="N4" s="4"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="70" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="52" t="s">
+      <c r="E5" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="53"/>
-      <c r="G5" s="62" t="s">
+      <c r="F5" s="63"/>
+      <c r="G5" s="72" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="63"/>
-      <c r="I5" s="66" t="s">
+      <c r="H5" s="73"/>
+      <c r="I5" s="76" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="68" t="s">
+      <c r="J5" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="64" t="s">
+      <c r="K5" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="57"/>
-      <c r="M5" s="60"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="71"/>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="30"/>
+      <c r="L5" s="67"/>
+      <c r="M5" s="70"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="51"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="49"/>
       <c r="E6" s="14" t="s">
         <v>21</v>
       </c>
@@ -2141,19 +2242,23 @@
       <c r="H6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="67"/>
-      <c r="J6" s="69"/>
-      <c r="K6" s="65"/>
-      <c r="L6" s="58"/>
-      <c r="M6" s="61"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I6" s="77"/>
+      <c r="J6" s="79"/>
+      <c r="K6" s="75"/>
+      <c r="L6" s="68"/>
+      <c r="M6" s="71"/>
+    </row>
+    <row r="7" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A7" s="11"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
+      <c r="E7" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="F7" s="80" t="s">
+        <v>93</v>
+      </c>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
@@ -2164,7 +2269,7 @@
       <c r="L7" s="12"/>
       <c r="M7" s="13"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="11"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -2181,7 +2286,7 @@
       <c r="L8" s="12"/>
       <c r="M8" s="13"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="11"/>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
@@ -2198,127 +2303,9 @@
       <c r="L9" s="12"/>
       <c r="M9" s="13"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="13"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="13"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="13"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="13"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="13"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
-      <c r="J15" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="13"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="11"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
-      <c r="J16" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="13"/>
-    </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="D5:D6"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="C5:C6"/>
@@ -2335,7 +2322,6 @@
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="I5:I6"/>
     <mergeCell ref="J5:J6"/>
-    <mergeCell ref="D5:D6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{08B9185A-577F-48B9-9ED8-67B0BBF2A510}"/>
@@ -2351,111 +2337,111 @@
   <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:M2"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="18.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="43.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="18.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="43.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="38" style="1" customWidth="1"/>
-    <col min="13" max="13" width="46.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="132.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="50.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="66.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="52.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.42578125" style="1"/>
+    <col min="13" max="13" width="46.33203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="132.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="50.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="66.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="52.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="40" t="str">
-        <f>'[1]Listado Objetos de Dominio'!A6</f>
+      <c r="B2" s="43" t="str">
+        <f>'[2]Listado Objetos de Dominio'!A6</f>
         <v>Administrador</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="41"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="44"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="25" t="str">
+      <c r="B3" s="45" t="str">
         <f>'Listado Objetos de Dominio'!$B$5</f>
         <v>Objeto de dominio que representa a cada una de las zonas comunes que se encuentran dentro de un conjunto residencial para que los residentes puedan reservar esos espacios y porder usarlos.</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="26"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="45"/>
+      <c r="M3" s="46"/>
       <c r="N3" s="4"/>
     </row>
-    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="27"/>
+      <c r="C4" s="35"/>
       <c r="D4" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="28"/>
-      <c r="G4" s="35" t="s">
+      <c r="F4" s="47"/>
+      <c r="G4" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="35"/>
+      <c r="H4" s="38"/>
       <c r="I4" s="9" t="s">
         <v>14</v>
       </c>
@@ -2465,52 +2451,52 @@
       <c r="K4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="38" t="s">
+      <c r="L4" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="39" t="s">
+      <c r="M4" s="42" t="s">
         <v>18</v>
       </c>
       <c r="N4" s="4"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="28"/>
-      <c r="G5" s="33" t="s">
+      <c r="F5" s="47"/>
+      <c r="G5" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="33"/>
-      <c r="I5" s="36" t="s">
+      <c r="H5" s="36"/>
+      <c r="I5" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="37" t="s">
+      <c r="J5" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="34" t="s">
+      <c r="K5" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="38"/>
-      <c r="M5" s="39"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="30"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="42"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="34"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="49"/>
       <c r="E6" s="14" t="s">
         <v>21</v>
       </c>
@@ -2523,13 +2509,13 @@
       <c r="H6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="36"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="39"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I6" s="39"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="42"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="11"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
@@ -2540,13 +2526,13 @@
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
       <c r="M7" s="13"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="11"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -2557,13 +2543,13 @@
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
       <c r="J8" s="12" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
       <c r="M8" s="13"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="11"/>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
@@ -2574,13 +2560,13 @@
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
       <c r="J9" s="12" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
       <c r="M9" s="13"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="11"/>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
@@ -2591,13 +2577,13 @@
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
       <c r="J10" s="12" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
       <c r="M10" s="13"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="11"/>
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
@@ -2608,13 +2594,13 @@
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
       <c r="J11" s="12" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
       <c r="M11" s="13"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="11"/>
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
@@ -2625,13 +2611,13 @@
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
       <c r="J12" s="12" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
       <c r="M12" s="13"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="11"/>
       <c r="B13" s="12"/>
       <c r="C13" s="12"/>
@@ -2642,7 +2628,7 @@
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
       <c r="J13" s="12" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
@@ -2650,6 +2636,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="D5:D6"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="B2:M2"/>
     <mergeCell ref="B3:M3"/>
@@ -2666,7 +2653,6 @@
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="K5:K6"/>
-    <mergeCell ref="D5:D6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{6A881977-C9D3-4BAB-A0CB-AD08821793D2}"/>
@@ -2682,112 +2668,112 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{135EFB96-F09D-4669-AFCD-45B4BA78057C}">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:N1"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7:F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="18.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="28.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="18.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15.44140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.21875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="28.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="38" style="1" customWidth="1"/>
-    <col min="13" max="13" width="46.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="132.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="50.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="66.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="52.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.42578125" style="1"/>
+    <col min="13" max="13" width="46.33203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="132.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="50.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="66.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="52.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="40" t="str">
-        <f>'[1]Listado Objetos de Dominio'!A7</f>
+      <c r="B2" s="43" t="str">
+        <f>'[2]Listado Objetos de Dominio'!A7</f>
         <v>Agenda</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="41"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="44"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="25" t="str">
+      <c r="B3" s="45" t="str">
         <f>'Listado Objetos de Dominio'!$B$5</f>
         <v>Objeto de dominio que representa a cada una de las zonas comunes que se encuentran dentro de un conjunto residencial para que los residentes puedan reservar esos espacios y porder usarlos.</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="26"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="45"/>
+      <c r="M3" s="46"/>
       <c r="N3" s="4"/>
     </row>
-    <row r="4" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="27"/>
+      <c r="C4" s="35"/>
       <c r="D4" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="28"/>
-      <c r="G4" s="35" t="s">
+      <c r="F4" s="47"/>
+      <c r="G4" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="35"/>
+      <c r="H4" s="38"/>
       <c r="I4" s="9" t="s">
         <v>14</v>
       </c>
@@ -2797,52 +2783,52 @@
       <c r="K4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="38" t="s">
+      <c r="L4" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="39" t="s">
+      <c r="M4" s="42" t="s">
         <v>18</v>
       </c>
       <c r="N4" s="4"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="27" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="28"/>
-      <c r="G5" s="33" t="s">
+      <c r="F5" s="47"/>
+      <c r="G5" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="33"/>
-      <c r="I5" s="36" t="s">
+      <c r="H5" s="36"/>
+      <c r="I5" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="37" t="s">
+      <c r="J5" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="34" t="s">
+      <c r="K5" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="38"/>
-      <c r="M5" s="39"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="30"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="42"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="34"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="49"/>
       <c r="E6" s="14" t="s">
         <v>21</v>
       </c>
@@ -2855,133 +2841,217 @@
       <c r="H6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="36"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="39"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="13"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="11"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="13"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="42"/>
+    </row>
+    <row r="7" spans="1:14" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="83" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="85" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="89" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="83" t="s">
+        <v>94</v>
+      </c>
+      <c r="F7" s="85" t="s">
+        <v>95</v>
+      </c>
+      <c r="G7" s="83" t="s">
+        <v>80</v>
+      </c>
+      <c r="H7" s="85" t="s">
+        <v>81</v>
+      </c>
+      <c r="I7" s="83"/>
+      <c r="J7" s="83" t="s">
+        <v>50</v>
+      </c>
+      <c r="K7" s="83"/>
+      <c r="L7" s="83"/>
+      <c r="M7" s="87"/>
+    </row>
+    <row r="8" spans="1:14" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="84"/>
+      <c r="C8" s="86"/>
+      <c r="D8" s="90"/>
+      <c r="E8" s="84"/>
+      <c r="F8" s="86"/>
+      <c r="G8" s="84"/>
+      <c r="H8" s="86"/>
+      <c r="I8" s="84"/>
+      <c r="J8" s="84"/>
+      <c r="K8" s="84"/>
+      <c r="L8" s="84"/>
+      <c r="M8" s="88"/>
+    </row>
+    <row r="9" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+      <c r="A9" s="81" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="83" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="85" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="83" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="83" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="85" t="s">
+        <v>91</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" s="80" t="s">
+        <v>82</v>
+      </c>
       <c r="I9" s="12"/>
-      <c r="J9" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="13"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="11"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
+      <c r="J9" s="83" t="s">
+        <v>67</v>
+      </c>
+      <c r="K9" s="83"/>
+      <c r="L9" s="83"/>
+      <c r="M9" s="87"/>
+    </row>
+    <row r="10" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="95"/>
+      <c r="B10" s="92"/>
+      <c r="C10" s="94"/>
+      <c r="D10" s="92"/>
+      <c r="E10" s="92"/>
+      <c r="F10" s="94"/>
+      <c r="G10" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="H10" s="80" t="s">
+        <v>85</v>
+      </c>
       <c r="I10" s="12"/>
-      <c r="J10" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="13"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
+      <c r="J10" s="92"/>
+      <c r="K10" s="92"/>
+      <c r="L10" s="92"/>
+      <c r="M10" s="96"/>
+    </row>
+    <row r="11" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+      <c r="A11" s="82"/>
+      <c r="B11" s="84"/>
+      <c r="C11" s="86"/>
+      <c r="D11" s="84"/>
+      <c r="E11" s="84"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="12" t="str">
+        <f>G9</f>
+        <v>Agenda-Pol-0002</v>
+      </c>
+      <c r="H11" s="80" t="s">
+        <v>82</v>
+      </c>
       <c r="I11" s="12"/>
-      <c r="J11" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="13"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
+      <c r="J11" s="84"/>
+      <c r="K11" s="84"/>
+      <c r="L11" s="84"/>
+      <c r="M11" s="88"/>
+    </row>
+    <row r="12" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="80" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="91" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="93" t="s">
+        <v>91</v>
+      </c>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
       <c r="I12" s="12"/>
       <c r="J12" s="12" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="K12" s="12"/>
       <c r="L12" s="12"/>
       <c r="M12" s="13"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
+    <row r="13" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="80" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="80" t="s">
+        <v>91</v>
+      </c>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
       <c r="I13" s="12"/>
       <c r="J13" s="12" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
       <c r="M13" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="39">
+    <mergeCell ref="K9:K11"/>
+    <mergeCell ref="L9:L11"/>
+    <mergeCell ref="M9:M11"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="J9:J11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="B2:M2"/>
@@ -2998,7 +3068,6 @@
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:I6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{175DFE60-DD9E-49DC-B6DD-E705858EF325}"/>
@@ -3017,108 +3086,108 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="18.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="28.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="18.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="28.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="38" style="1" customWidth="1"/>
-    <col min="13" max="13" width="46.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="132.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="50.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="66.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="52.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.42578125" style="1"/>
+    <col min="13" max="13" width="46.33203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="132.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="50.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="66.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="52.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="40" t="str">
-        <f>'[1]Listado Objetos de Dominio'!A7</f>
+      <c r="B2" s="43" t="str">
+        <f>'[2]Listado Objetos de Dominio'!A7</f>
         <v>Agenda</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="41"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="44"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="25" t="str">
+      <c r="B3" s="45" t="str">
         <f>'Listado Objetos de Dominio'!$B$5</f>
         <v>Objeto de dominio que representa a cada una de las zonas comunes que se encuentran dentro de un conjunto residencial para que los residentes puedan reservar esos espacios y porder usarlos.</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="26"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="45"/>
+      <c r="M3" s="46"/>
       <c r="N3" s="4"/>
     </row>
-    <row r="4" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="27"/>
+      <c r="C4" s="35"/>
       <c r="D4" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="28"/>
-      <c r="G4" s="35" t="s">
+      <c r="F4" s="47"/>
+      <c r="G4" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="35"/>
+      <c r="H4" s="38"/>
       <c r="I4" s="9" t="s">
         <v>14</v>
       </c>
@@ -3128,52 +3197,52 @@
       <c r="K4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="38" t="s">
+      <c r="L4" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="39" t="s">
+      <c r="M4" s="42" t="s">
         <v>18</v>
       </c>
       <c r="N4" s="4"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="28"/>
-      <c r="G5" s="33" t="s">
+      <c r="F5" s="47"/>
+      <c r="G5" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="33"/>
-      <c r="I5" s="36" t="s">
+      <c r="H5" s="36"/>
+      <c r="I5" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="37" t="s">
+      <c r="J5" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="34" t="s">
+      <c r="K5" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="38"/>
-      <c r="M5" s="39"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="30"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="42"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="34"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="49"/>
       <c r="E6" s="14" t="s">
         <v>21</v>
       </c>
@@ -3186,13 +3255,13 @@
       <c r="H6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="36"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="39"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I6" s="39"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="42"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="11"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
@@ -3203,13 +3272,13 @@
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
       <c r="M7" s="13"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="11"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -3220,13 +3289,13 @@
       <c r="H8" s="12"/>
       <c r="I8" s="12"/>
       <c r="J8" s="12" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
       <c r="M8" s="13"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="11"/>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
@@ -3237,13 +3306,13 @@
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
       <c r="J9" s="12" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
       <c r="M9" s="13"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="11"/>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
@@ -3254,13 +3323,13 @@
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
       <c r="J10" s="12" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
       <c r="M10" s="13"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="11"/>
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
@@ -3271,7 +3340,7 @@
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
       <c r="J11" s="12" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
@@ -3279,6 +3348,7 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="I5:I6"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="B2:M2"/>
@@ -3295,7 +3365,6 @@
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:I6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{755244C2-D34A-4436-ABEF-3130787CFBF9}"/>
@@ -3308,114 +3377,114 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC47FB83-9179-46D6-840D-CDDDAC34ECFB}">
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
-    <col min="5" max="6" width="18.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.28515625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="34.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="18.88671875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="15" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="34.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="38" style="1" customWidth="1"/>
-    <col min="13" max="13" width="46.28515625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="132.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="50.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="66.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="52.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.42578125" style="1"/>
+    <col min="13" max="13" width="46.33203125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="132.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="50.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="66.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="52.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="40" t="str">
-        <f>'[1]Listado Objetos de Dominio'!A7</f>
+      <c r="B2" s="43" t="str">
+        <f>'[2]Listado Objetos de Dominio'!A7</f>
         <v>Agenda</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="41"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="44"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="25" t="str">
+      <c r="B3" s="45" t="str">
         <f>'Listado Objetos de Dominio'!$B$5</f>
         <v>Objeto de dominio que representa a cada una de las zonas comunes que se encuentran dentro de un conjunto residencial para que los residentes puedan reservar esos espacios y porder usarlos.</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="26"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="45"/>
+      <c r="M3" s="46"/>
       <c r="N3" s="4"/>
     </row>
-    <row r="4" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="27"/>
+      <c r="C4" s="35"/>
       <c r="D4" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="28"/>
-      <c r="G4" s="35" t="s">
+      <c r="F4" s="47"/>
+      <c r="G4" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="35"/>
+      <c r="H4" s="38"/>
       <c r="I4" s="9" t="s">
         <v>14</v>
       </c>
@@ -3425,52 +3494,52 @@
       <c r="K4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="38" t="s">
+      <c r="L4" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="39" t="s">
+      <c r="M4" s="42" t="s">
         <v>18</v>
       </c>
       <c r="N4" s="4"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="D5" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="28"/>
-      <c r="G5" s="33" t="s">
+      <c r="F5" s="47"/>
+      <c r="G5" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="33"/>
-      <c r="I5" s="36" t="s">
+      <c r="H5" s="36"/>
+      <c r="I5" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="37" t="s">
+      <c r="J5" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="34" t="s">
+      <c r="K5" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="38"/>
-      <c r="M5" s="39"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="32"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="30"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="42"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="34"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="49"/>
       <c r="E6" s="14" t="s">
         <v>21</v>
       </c>
@@ -3483,47 +3552,53 @@
       <c r="H6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="36"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="34"/>
-      <c r="L6" s="38"/>
-      <c r="M6" s="39"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I6" s="39"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="42"/>
+    </row>
+    <row r="7" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A7" s="11"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
+      <c r="G7" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="H7" s="80" t="s">
+        <v>88</v>
+      </c>
       <c r="I7" s="12"/>
       <c r="J7" s="12" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
       <c r="M7" s="13"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="11"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
+      <c r="G8" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="H8" s="80" t="s">
+        <v>90</v>
+      </c>
       <c r="I8" s="12"/>
-      <c r="J8" s="12" t="s">
-        <v>70</v>
-      </c>
+      <c r="J8" s="12"/>
       <c r="K8" s="12"/>
       <c r="L8" s="12"/>
       <c r="M8" s="13"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="11"/>
       <c r="B9" s="12"/>
       <c r="C9" s="12"/>
@@ -3534,13 +3609,13 @@
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
       <c r="J9" s="12" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
       <c r="M9" s="13"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="11"/>
       <c r="B10" s="12"/>
       <c r="C10" s="12"/>
@@ -3551,48 +3626,15 @@
       <c r="H10" s="12"/>
       <c r="I10" s="12"/>
       <c r="J10" s="12" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
       <c r="M10" s="13"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="11"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="13"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="11"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="13"/>
-    </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="I5:I6"/>
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="B2:M2"/>
@@ -3609,7 +3651,6 @@
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:I6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{72BB53BB-A255-4E65-8E13-6A32013B466E}"/>
@@ -3627,6 +3668,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C279D002CEC08F42B7087C30E58D0266" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e5713f579c7011938dc4987ae8981b8f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3219184d-29ab-4105-b29c-8e343e335d59" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ae0a0ff84a3c6712467f60982d6e378d" ns2:_="">
     <xsd:import namespace="3219184d-29ab-4105-b29c-8e343e335d59"/>
@@ -3770,15 +3820,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2038022-656B-4A1B-A485-51A1972238BD}">
   <ds:schemaRefs>
@@ -3797,6 +3838,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6724C681-8A04-4D66-BB1C-57F7466573C0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8AEECCE0-61F9-4782-94C5-382F8EFF459D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3814,14 +3863,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6724C681-8A04-4D66-BB1C-57F7466573C0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{6ebbfa72-b3b6-4c1f-8b23-058d4f67f013}" enabled="1" method="Privileged" siteId="{bf1ce8b5-5d39-4bc5-ad6e-07b3e4d7d67a}" contentBits="0" removed="0"/>

</xml_diff>

<commit_message>
Proyecto al dia termine Event storming de Residentes y de reservas y organize el Draw poniendo las relaciones entre contextos
</commit_message>
<xml_diff>
--- a/Doo-Doc/Seccion # 7/ConjuntosResidenciales - Event Storming.xlsx
+++ b/Doo-Doc/Seccion # 7/ConjuntosResidenciales - Event Storming.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uconet-my.sharepoint.com/personal/juan_avendano1956_uco_net_co/Documents/Documents/victus-doc/Doo-Doc/Seccion # 7/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\DOO 2024 BD\DOO\victus-doc\Doo-Doc\Seccion # 7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1213" documentId="13_ncr:1_{6A1F0B49-DD34-4DE4-8D57-041CC992534B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A90DADA1-56E2-4441-BB89-F5BB490E5F85}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F05F4909-7F27-4A2A-88DD-FA156467696E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="7" xr2:uid="{36012E7C-B3F4-482B-AC16-7CCB81B9AE88}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" firstSheet="3" activeTab="3" xr2:uid="{36012E7C-B3F4-482B-AC16-7CCB81B9AE88}"/>
   </bookViews>
   <sheets>
     <sheet name="Flujo de eventos en el tiempo" sheetId="61" r:id="rId1"/>
@@ -1250,6 +1250,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1274,6 +1283,30 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1319,10 +1352,31 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1415,67 +1469,13 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1575,10 +1575,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1882,15 +1878,15 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="11.44140625" style="2"/>
+    <col min="1" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1"/>
     </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F18"/>
     </row>
   </sheetData>
@@ -1909,35 +1905,35 @@
       <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.5546875" customWidth="1"/>
-    <col min="2" max="2" width="50.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" customWidth="1"/>
-    <col min="4" max="4" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="38"/>
-    </row>
-    <row r="2" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="40"/>
+      <c r="D1" s="41"/>
+    </row>
+    <row r="2" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="39" t="s">
+      <c r="B2" s="42" t="s">
         <v>139</v>
       </c>
-      <c r="C2" s="40"/>
-      <c r="D2" s="41"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>4</v>
       </c>
@@ -1951,7 +1947,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="42" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>29</v>
       </c>
@@ -1961,12 +1957,12 @@
       <c r="C4" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="42" t="str">
+      <c r="D4" s="45" t="str">
         <f>$B$1</f>
         <v>Gestión de conjuntos residenciales</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="64.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="64.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
         <v>30</v>
       </c>
@@ -1976,9 +1972,9 @@
       <c r="C5" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="43"/>
-    </row>
-    <row r="6" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="46"/>
+    </row>
+    <row r="6" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
         <v>31</v>
       </c>
@@ -1988,9 +1984,9 @@
       <c r="C6" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="43"/>
-    </row>
-    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D6" s="46"/>
+    </row>
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
         <v>32</v>
       </c>
@@ -2000,9 +1996,9 @@
       <c r="C7" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="43"/>
-    </row>
-    <row r="8" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D7" s="46"/>
+    </row>
+    <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
         <v>33</v>
       </c>
@@ -2012,9 +2008,9 @@
       <c r="C8" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="43"/>
-    </row>
-    <row r="9" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D8" s="46"/>
+    </row>
+    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
         <v>57</v>
       </c>
@@ -2024,7 +2020,7 @@
       <c r="C9" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="44"/>
+      <c r="D9" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2049,111 +2045,111 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{235BA608-57CC-45B0-8234-10CA49C3B004}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="18.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.109375" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="28.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="18.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="28.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="38" style="1" customWidth="1"/>
-    <col min="13" max="13" width="46.33203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="132.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="50.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="66.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="52.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.44140625" style="1"/>
+    <col min="13" max="13" width="46.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="132.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="50.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="66.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="52.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="59"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="69"/>
+      <c r="M2" s="70"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="60" t="str">
+      <c r="B3" s="54" t="str">
         <f>'Listado Objetos de Dominio'!B4</f>
         <v>Objeto de dominio que representa a cada uno de los conjuntos residenciales existentes.</v>
       </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="61"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="55"/>
       <c r="N3" s="4"/>
     </row>
-    <row r="4" spans="1:14" ht="29.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="45"/>
+      <c r="C4" s="56"/>
       <c r="D4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="46" t="s">
+      <c r="E4" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="46"/>
-      <c r="G4" s="53" t="s">
+      <c r="F4" s="57"/>
+      <c r="G4" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="53"/>
+      <c r="H4" s="64"/>
       <c r="I4" s="9" t="s">
         <v>14</v>
       </c>
@@ -2163,52 +2159,52 @@
       <c r="K4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="56" t="s">
+      <c r="L4" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="57" t="s">
+      <c r="M4" s="68" t="s">
         <v>18</v>
       </c>
       <c r="N4" s="4"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="50" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="47" t="s">
+      <c r="D5" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="46"/>
-      <c r="G5" s="51" t="s">
+      <c r="F5" s="57"/>
+      <c r="G5" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="51"/>
-      <c r="I5" s="54" t="s">
+      <c r="H5" s="62"/>
+      <c r="I5" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="55" t="s">
+      <c r="J5" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="52" t="s">
+      <c r="K5" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="56"/>
-      <c r="M5" s="57"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="50"/>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="48"/>
+      <c r="L5" s="67"/>
+      <c r="M5" s="68"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="61"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="59"/>
       <c r="E6" s="11" t="s">
         <v>21</v>
       </c>
@@ -2221,198 +2217,198 @@
       <c r="H6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="54"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="57"/>
-    </row>
-    <row r="7" spans="1:14" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="98" t="s">
+      <c r="I6" s="65"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="67"/>
+      <c r="M6" s="68"/>
+    </row>
+    <row r="7" spans="1:14" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="B7" s="92" t="s">
+      <c r="B7" s="48" t="s">
         <v>84</v>
       </c>
-      <c r="C7" s="92" t="s">
+      <c r="C7" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="D7" s="92" t="s">
+      <c r="D7" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="92"/>
-      <c r="F7" s="92"/>
-      <c r="G7" s="92" t="s">
+      <c r="E7" s="48"/>
+      <c r="F7" s="48"/>
+      <c r="G7" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="H7" s="92" t="s">
+      <c r="H7" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="I7" s="92"/>
-      <c r="J7" s="92" t="s">
+      <c r="I7" s="48"/>
+      <c r="J7" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="K7" s="92"/>
-      <c r="L7" s="92" t="s">
+      <c r="K7" s="48"/>
+      <c r="L7" s="48" t="s">
         <v>38</v>
       </c>
       <c r="M7" s="28" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="100"/>
-      <c r="B8" s="101"/>
-      <c r="C8" s="101"/>
-      <c r="D8" s="101"/>
-      <c r="E8" s="101"/>
-      <c r="F8" s="101"/>
-      <c r="G8" s="101"/>
-      <c r="H8" s="101"/>
-      <c r="I8" s="101"/>
-      <c r="J8" s="101"/>
-      <c r="K8" s="101"/>
-      <c r="L8" s="101"/>
+    <row r="8" spans="1:14" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="52"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="49"/>
+      <c r="K8" s="49"/>
+      <c r="L8" s="49"/>
       <c r="M8" s="28" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="100"/>
-      <c r="B9" s="101"/>
-      <c r="C9" s="101"/>
-      <c r="D9" s="101"/>
-      <c r="E9" s="101"/>
-      <c r="F9" s="101"/>
-      <c r="G9" s="101"/>
-      <c r="H9" s="101"/>
-      <c r="I9" s="101"/>
-      <c r="J9" s="101"/>
-      <c r="K9" s="101"/>
-      <c r="L9" s="101"/>
+    <row r="9" spans="1:14" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="52"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
+      <c r="H9" s="49"/>
+      <c r="I9" s="49"/>
+      <c r="J9" s="49"/>
+      <c r="K9" s="49"/>
+      <c r="L9" s="49"/>
       <c r="M9" s="28" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="100"/>
-      <c r="B10" s="101"/>
-      <c r="C10" s="101"/>
-      <c r="D10" s="101"/>
-      <c r="E10" s="101"/>
-      <c r="F10" s="101"/>
-      <c r="G10" s="101"/>
-      <c r="H10" s="101"/>
-      <c r="I10" s="101"/>
-      <c r="J10" s="101"/>
-      <c r="K10" s="101"/>
-      <c r="L10" s="101"/>
+    <row r="10" spans="1:14" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="52"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="49"/>
+      <c r="L10" s="49"/>
       <c r="M10" s="28" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="99"/>
-      <c r="B11" s="93"/>
-      <c r="C11" s="93"/>
-      <c r="D11" s="93"/>
-      <c r="E11" s="93"/>
-      <c r="F11" s="93"/>
-      <c r="G11" s="93"/>
-      <c r="H11" s="93"/>
-      <c r="I11" s="93"/>
-      <c r="J11" s="93"/>
-      <c r="K11" s="93"/>
-      <c r="L11" s="93"/>
+    <row r="11" spans="1:14" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="53"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="50"/>
       <c r="M11" s="28" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="98" t="s">
+    <row r="12" spans="1:14" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="B12" s="92" t="s">
+      <c r="B12" s="48" t="s">
         <v>87</v>
       </c>
-      <c r="C12" s="92" t="s">
+      <c r="C12" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="D12" s="92" t="s">
+      <c r="D12" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="92"/>
-      <c r="F12" s="92"/>
-      <c r="G12" s="92" t="s">
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="H12" s="92" t="s">
+      <c r="H12" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="I12" s="92"/>
-      <c r="J12" s="92" t="s">
+      <c r="I12" s="48"/>
+      <c r="J12" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="K12" s="92"/>
-      <c r="L12" s="92" t="s">
+      <c r="K12" s="48"/>
+      <c r="L12" s="48" t="s">
         <v>81</v>
       </c>
       <c r="M12" s="28" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="100"/>
-      <c r="B13" s="101"/>
-      <c r="C13" s="101"/>
-      <c r="D13" s="101"/>
-      <c r="E13" s="101"/>
-      <c r="F13" s="101"/>
-      <c r="G13" s="101"/>
-      <c r="H13" s="101"/>
-      <c r="I13" s="101"/>
-      <c r="J13" s="101"/>
-      <c r="K13" s="101"/>
-      <c r="L13" s="101"/>
+    <row r="13" spans="1:14" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="52"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="49"/>
+      <c r="L13" s="49"/>
       <c r="M13" s="28" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="100"/>
-      <c r="B14" s="101"/>
-      <c r="C14" s="101"/>
-      <c r="D14" s="101"/>
-      <c r="E14" s="101"/>
-      <c r="F14" s="101"/>
-      <c r="G14" s="101"/>
-      <c r="H14" s="101"/>
-      <c r="I14" s="101"/>
-      <c r="J14" s="101"/>
-      <c r="K14" s="101"/>
-      <c r="L14" s="101"/>
+    <row r="14" spans="1:14" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="52"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="49"/>
+      <c r="K14" s="49"/>
+      <c r="L14" s="49"/>
       <c r="M14" s="28" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="99"/>
-      <c r="B15" s="93"/>
-      <c r="C15" s="93"/>
-      <c r="D15" s="93"/>
-      <c r="E15" s="93"/>
-      <c r="F15" s="93"/>
-      <c r="G15" s="93"/>
-      <c r="H15" s="93"/>
-      <c r="I15" s="93"/>
-      <c r="J15" s="93"/>
-      <c r="K15" s="93"/>
-      <c r="L15" s="93"/>
+    <row r="15" spans="1:14" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="53"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="50"/>
+      <c r="J15" s="50"/>
+      <c r="K15" s="50"/>
+      <c r="L15" s="50"/>
       <c r="M15" s="28" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="99.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="99.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
         <v>90</v>
       </c>
@@ -2445,7 +2441,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
         <v>83</v>
       </c>
@@ -2478,7 +2474,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
         <v>31</v>
       </c>
@@ -2511,7 +2507,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
         <v>31</v>
       </c>
@@ -2544,7 +2540,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="27" t="s">
         <v>83</v>
       </c>
@@ -2579,35 +2575,6 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="G12:G15"/>
-    <mergeCell ref="F12:F15"/>
-    <mergeCell ref="E12:E15"/>
-    <mergeCell ref="D12:D15"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="L12:L15"/>
-    <mergeCell ref="K12:K15"/>
-    <mergeCell ref="J12:J15"/>
-    <mergeCell ref="I12:I15"/>
-    <mergeCell ref="H12:H15"/>
-    <mergeCell ref="L7:L11"/>
-    <mergeCell ref="K7:K11"/>
-    <mergeCell ref="J7:J11"/>
-    <mergeCell ref="I7:I11"/>
-    <mergeCell ref="H7:H11"/>
-    <mergeCell ref="G7:G11"/>
-    <mergeCell ref="F7:F11"/>
-    <mergeCell ref="E7:E11"/>
-    <mergeCell ref="D7:D11"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="B7:B11"/>
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="D5:D6"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="A5:A6"/>
     <mergeCell ref="B5:B6"/>
@@ -2620,6 +2587,35 @@
     <mergeCell ref="L4:L6"/>
     <mergeCell ref="M4:M6"/>
     <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="G7:G11"/>
+    <mergeCell ref="F7:F11"/>
+    <mergeCell ref="E7:E11"/>
+    <mergeCell ref="D7:D11"/>
+    <mergeCell ref="C7:C11"/>
+    <mergeCell ref="L7:L11"/>
+    <mergeCell ref="K7:K11"/>
+    <mergeCell ref="J7:J11"/>
+    <mergeCell ref="I7:I11"/>
+    <mergeCell ref="H7:H11"/>
+    <mergeCell ref="L12:L15"/>
+    <mergeCell ref="K12:K15"/>
+    <mergeCell ref="J12:J15"/>
+    <mergeCell ref="I12:I15"/>
+    <mergeCell ref="H12:H15"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="G12:G15"/>
+    <mergeCell ref="F12:F15"/>
+    <mergeCell ref="E12:E15"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="C12:C15"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
@@ -2636,113 +2632,113 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9732BFC6-5B3A-4E40-BEA3-58E7EDB79B0C}">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.21875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="27.44140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.5546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="37.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="27.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="37.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="38" style="1" customWidth="1"/>
-    <col min="13" max="13" width="46.33203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="132.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="50.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="66.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="52.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.44140625" style="1"/>
+    <col min="13" max="13" width="46.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="132.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="50.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="66.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="52.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="64" t="s">
+      <c r="B2" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="66"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="84"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="67" t="str">
+      <c r="B3" s="85" t="str">
         <f>'Listado Objetos de Dominio'!$B$5</f>
         <v>Objeto de dominio que representa a cada una de las zonas comunes que se encuentran dentro de un conjunto residencial para que los residentes puedan reservar esos espacios y porder usarlos.</v>
       </c>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
-      <c r="H3" s="68"/>
-      <c r="I3" s="68"/>
-      <c r="J3" s="68"/>
-      <c r="K3" s="68"/>
-      <c r="L3" s="68"/>
-      <c r="M3" s="69"/>
+      <c r="C3" s="86"/>
+      <c r="D3" s="86"/>
+      <c r="E3" s="86"/>
+      <c r="F3" s="86"/>
+      <c r="G3" s="86"/>
+      <c r="H3" s="86"/>
+      <c r="I3" s="86"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="86"/>
+      <c r="L3" s="86"/>
+      <c r="M3" s="87"/>
       <c r="N3" s="4"/>
     </row>
-    <row r="4" spans="1:14" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="70" t="s">
+      <c r="B4" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="71"/>
+      <c r="C4" s="89"/>
       <c r="D4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="72" t="s">
+      <c r="E4" s="90" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="73"/>
-      <c r="G4" s="74" t="s">
+      <c r="F4" s="91"/>
+      <c r="G4" s="92" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="75"/>
+      <c r="H4" s="93"/>
       <c r="I4" s="9" t="s">
         <v>14</v>
       </c>
@@ -2752,52 +2748,52 @@
       <c r="K4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="76" t="s">
+      <c r="L4" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="79" t="s">
+      <c r="M4" s="97" t="s">
         <v>18</v>
       </c>
       <c r="N4" s="4"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="90" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="108" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="62" t="s">
+      <c r="B5" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="62" t="s">
+      <c r="C5" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="47" t="s">
+      <c r="D5" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="72" t="s">
+      <c r="E5" s="90" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="73"/>
-      <c r="G5" s="82" t="s">
+      <c r="F5" s="91"/>
+      <c r="G5" s="100" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="83"/>
-      <c r="I5" s="86" t="s">
+      <c r="H5" s="101"/>
+      <c r="I5" s="104" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="88" t="s">
+      <c r="J5" s="106" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="84" t="s">
+      <c r="K5" s="102" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="77"/>
-      <c r="M5" s="80"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="91"/>
-      <c r="B6" s="63"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="48"/>
+      <c r="L5" s="95"/>
+      <c r="M5" s="98"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="109"/>
+      <c r="B6" s="81"/>
+      <c r="C6" s="81"/>
+      <c r="D6" s="59"/>
       <c r="E6" s="11" t="s">
         <v>21</v>
       </c>
@@ -2810,29 +2806,29 @@
       <c r="H6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="87"/>
-      <c r="J6" s="89"/>
-      <c r="K6" s="85"/>
-      <c r="L6" s="78"/>
-      <c r="M6" s="81"/>
-    </row>
-    <row r="7" spans="1:14" ht="88.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="103" t="s">
+      <c r="I6" s="105"/>
+      <c r="J6" s="107"/>
+      <c r="K6" s="103"/>
+      <c r="L6" s="96"/>
+      <c r="M6" s="99"/>
+    </row>
+    <row r="7" spans="1:14" ht="88.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="71" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="94" t="s">
+      <c r="B7" s="74" t="s">
         <v>105</v>
       </c>
-      <c r="C7" s="94" t="s">
+      <c r="C7" s="74" t="s">
         <v>106</v>
       </c>
-      <c r="D7" s="94" t="s">
+      <c r="D7" s="74" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="94" t="s">
+      <c r="E7" s="74" t="s">
         <v>104</v>
       </c>
-      <c r="F7" s="94" t="s">
+      <c r="F7" s="74" t="s">
         <v>103</v>
       </c>
       <c r="G7" s="24" t="s">
@@ -2841,129 +2837,129 @@
       <c r="H7" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="I7" s="94"/>
-      <c r="J7" s="94" t="s">
+      <c r="I7" s="74"/>
+      <c r="J7" s="74" t="s">
         <v>39</v>
       </c>
-      <c r="K7" s="94"/>
-      <c r="L7" s="94" t="s">
+      <c r="K7" s="74"/>
+      <c r="L7" s="74" t="s">
         <v>40</v>
       </c>
       <c r="M7" s="26" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="106"/>
-      <c r="B8" s="105"/>
-      <c r="C8" s="105"/>
-      <c r="D8" s="105"/>
-      <c r="E8" s="105"/>
-      <c r="F8" s="105"/>
-      <c r="G8" s="94" t="s">
+    <row r="8" spans="1:14" ht="58.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="72"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="74" t="s">
         <v>113</v>
       </c>
-      <c r="H8" s="94" t="s">
+      <c r="H8" s="74" t="s">
         <v>162</v>
       </c>
-      <c r="I8" s="105"/>
-      <c r="J8" s="105"/>
-      <c r="K8" s="105"/>
-      <c r="L8" s="105"/>
-      <c r="M8" s="108" t="s">
+      <c r="I8" s="76"/>
+      <c r="J8" s="76"/>
+      <c r="K8" s="76"/>
+      <c r="L8" s="76"/>
+      <c r="M8" s="38" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="104"/>
-      <c r="B9" s="95"/>
-      <c r="C9" s="95"/>
-      <c r="D9" s="95"/>
-      <c r="E9" s="95"/>
-      <c r="F9" s="95"/>
-      <c r="G9" s="95"/>
-      <c r="H9" s="95"/>
-      <c r="I9" s="95"/>
-      <c r="J9" s="95"/>
-      <c r="K9" s="95"/>
-      <c r="L9" s="95"/>
-      <c r="M9" s="107" t="s">
+    <row r="9" spans="1:14" ht="58.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="73"/>
+      <c r="B9" s="75"/>
+      <c r="C9" s="75"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="75"/>
+      <c r="H9" s="75"/>
+      <c r="I9" s="75"/>
+      <c r="J9" s="75"/>
+      <c r="K9" s="75"/>
+      <c r="L9" s="75"/>
+      <c r="M9" s="37" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="B10" s="92" t="s">
+      <c r="B10" s="48" t="s">
         <v>109</v>
       </c>
-      <c r="C10" s="92" t="s">
+      <c r="C10" s="48" t="s">
         <v>110</v>
       </c>
-      <c r="D10" s="92" t="s">
+      <c r="D10" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="92" t="s">
+      <c r="E10" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="F10" s="92" t="s">
+      <c r="F10" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="G10" s="92" t="s">
+      <c r="G10" s="48" t="s">
         <v>107</v>
       </c>
-      <c r="H10" s="92" t="s">
+      <c r="H10" s="48" t="s">
         <v>111</v>
       </c>
-      <c r="I10" s="92"/>
-      <c r="J10" s="92" t="s">
+      <c r="I10" s="48"/>
+      <c r="J10" s="48" t="s">
         <v>108</v>
       </c>
-      <c r="K10" s="92"/>
-      <c r="L10" s="92" t="s">
+      <c r="K10" s="48"/>
+      <c r="L10" s="48" t="s">
         <v>39</v>
       </c>
       <c r="M10" s="26" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="60.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="93"/>
-      <c r="C11" s="93"/>
-      <c r="D11" s="93"/>
-      <c r="E11" s="93"/>
-      <c r="F11" s="93"/>
-      <c r="G11" s="93"/>
-      <c r="H11" s="93"/>
-      <c r="I11" s="93"/>
-      <c r="J11" s="93"/>
-      <c r="K11" s="93"/>
-      <c r="L11" s="93"/>
-      <c r="M11" s="108" t="s">
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="50"/>
+      <c r="M11" s="38" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="111" t="s">
+    <row r="12" spans="1:14" ht="86.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="78" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="92" t="s">
+      <c r="B12" s="48" t="s">
         <v>158</v>
       </c>
-      <c r="C12" s="92" t="s">
+      <c r="C12" s="48" t="s">
         <v>159</v>
       </c>
-      <c r="D12" s="92" t="s">
+      <c r="D12" s="48" t="s">
         <v>160</v>
       </c>
-      <c r="E12" s="92" t="s">
+      <c r="E12" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="F12" s="92" t="s">
+      <c r="F12" s="48" t="s">
         <v>161</v>
       </c>
       <c r="G12" s="24" t="s">
@@ -2972,54 +2968,54 @@
       <c r="H12" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="I12" s="92"/>
-      <c r="J12" s="92" t="s">
+      <c r="I12" s="48"/>
+      <c r="J12" s="48" t="s">
         <v>157</v>
       </c>
-      <c r="K12" s="92"/>
-      <c r="L12" s="92" t="s">
+      <c r="K12" s="48"/>
+      <c r="L12" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="M12" s="92" t="s">
+      <c r="M12" s="48" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="98.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="112"/>
-      <c r="B13" s="93"/>
-      <c r="C13" s="93"/>
-      <c r="D13" s="93"/>
-      <c r="E13" s="93"/>
-      <c r="F13" s="93"/>
+    <row r="13" spans="1:14" ht="98.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="79"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
       <c r="G13" s="21" t="s">
         <v>113</v>
       </c>
       <c r="H13" s="21" t="s">
         <v>162</v>
       </c>
-      <c r="I13" s="93"/>
-      <c r="J13" s="93"/>
-      <c r="K13" s="93"/>
-      <c r="L13" s="93"/>
-      <c r="M13" s="93"/>
-    </row>
-    <row r="14" spans="1:14" ht="120.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="110" t="s">
+      <c r="I13" s="50"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="50"/>
+      <c r="M13" s="50"/>
+    </row>
+    <row r="14" spans="1:14" ht="120.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="77" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="110" t="s">
+      <c r="B14" s="77" t="s">
         <v>114</v>
       </c>
-      <c r="C14" s="110" t="s">
+      <c r="C14" s="77" t="s">
         <v>115</v>
       </c>
-      <c r="D14" s="110" t="s">
+      <c r="D14" s="77" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="110" t="s">
+      <c r="E14" s="77" t="s">
         <v>104</v>
       </c>
-      <c r="F14" s="110" t="s">
+      <c r="F14" s="77" t="s">
         <v>116</v>
       </c>
       <c r="G14" s="24" t="s">
@@ -3028,50 +3024,74 @@
       <c r="H14" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="I14" s="110"/>
-      <c r="J14" s="110" t="s">
+      <c r="I14" s="77"/>
+      <c r="J14" s="77" t="s">
         <v>40</v>
       </c>
-      <c r="K14" s="110"/>
-      <c r="L14" s="110" t="s">
+      <c r="K14" s="77"/>
+      <c r="L14" s="77" t="s">
         <v>39</v>
       </c>
-      <c r="M14" s="110" t="s">
+      <c r="M14" s="77" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="110"/>
-      <c r="B15" s="110"/>
-      <c r="C15" s="110"/>
-      <c r="D15" s="110"/>
-      <c r="E15" s="110"/>
-      <c r="F15" s="110"/>
+    <row r="15" spans="1:14" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="77"/>
+      <c r="B15" s="77"/>
+      <c r="C15" s="77"/>
+      <c r="D15" s="77"/>
+      <c r="E15" s="77"/>
+      <c r="F15" s="77"/>
       <c r="G15" s="24" t="s">
         <v>117</v>
       </c>
       <c r="H15" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="I15" s="110"/>
-      <c r="J15" s="110"/>
-      <c r="K15" s="110"/>
-      <c r="L15" s="110"/>
-      <c r="M15" s="110"/>
+      <c r="I15" s="77"/>
+      <c r="J15" s="77"/>
+      <c r="K15" s="77"/>
+      <c r="L15" s="77"/>
+      <c r="M15" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="62">
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="L7:L9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="J7:J9"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="J14:J15"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
     <mergeCell ref="K14:K15"/>
     <mergeCell ref="L14:L15"/>
     <mergeCell ref="M14:M15"/>
@@ -3088,41 +3108,17 @@
     <mergeCell ref="M12:M13"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="L4:L6"/>
-    <mergeCell ref="M4:M6"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="L7:L9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="J7:J9"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="C7:C9"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
@@ -3138,111 +3134,111 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C3D88CD-1BA6-4157-9522-8201A0FEDE3C}">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:M13"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="18.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="43.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="18.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="43.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="38" style="1" customWidth="1"/>
-    <col min="13" max="13" width="46.33203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="132.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="50.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="66.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="52.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.44140625" style="1"/>
+    <col min="13" max="13" width="46.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="132.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="50.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="66.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="52.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="59"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="69"/>
+      <c r="M2" s="70"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="60" t="str">
+      <c r="B3" s="54" t="str">
         <f>'Listado Objetos de Dominio'!$B$6</f>
         <v xml:space="preserve"> Objeto de dominio que representa el Administrador encargado de hacer CRUD a zonas comunes y Usuarios(residentes), tambien encargado de cancelar reservas.</v>
       </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="61"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="55"/>
       <c r="N3" s="4"/>
     </row>
-    <row r="4" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="45"/>
+      <c r="C4" s="56"/>
       <c r="D4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="46" t="s">
+      <c r="E4" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="46"/>
-      <c r="G4" s="53" t="s">
+      <c r="F4" s="57"/>
+      <c r="G4" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="53"/>
+      <c r="H4" s="64"/>
       <c r="I4" s="9" t="s">
         <v>14</v>
       </c>
@@ -3252,52 +3248,52 @@
       <c r="K4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="56" t="s">
+      <c r="L4" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="57" t="s">
+      <c r="M4" s="68" t="s">
         <v>18</v>
       </c>
       <c r="N4" s="4"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="50" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="47" t="s">
+      <c r="D5" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="46"/>
-      <c r="G5" s="51" t="s">
+      <c r="F5" s="57"/>
+      <c r="G5" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="51"/>
-      <c r="I5" s="54" t="s">
+      <c r="H5" s="62"/>
+      <c r="I5" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="55" t="s">
+      <c r="J5" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="52" t="s">
+      <c r="K5" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="56"/>
-      <c r="M5" s="57"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="50"/>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="48"/>
+      <c r="L5" s="67"/>
+      <c r="M5" s="68"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="61"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="59"/>
       <c r="E6" s="11" t="s">
         <v>21</v>
       </c>
@@ -3310,84 +3306,84 @@
       <c r="H6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="54"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="57"/>
-    </row>
-    <row r="7" spans="1:14" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="98" t="s">
+      <c r="I6" s="65"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="67"/>
+      <c r="M6" s="68"/>
+    </row>
+    <row r="7" spans="1:14" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="B7" s="92" t="s">
+      <c r="B7" s="48" t="s">
         <v>119</v>
       </c>
-      <c r="C7" s="92" t="s">
+      <c r="C7" s="48" t="s">
         <v>120</v>
       </c>
-      <c r="D7" s="92" t="s">
+      <c r="D7" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="92" t="s">
+      <c r="E7" s="48" t="s">
         <v>121</v>
       </c>
-      <c r="F7" s="92" t="s">
+      <c r="F7" s="48" t="s">
         <v>122</v>
       </c>
-      <c r="G7" s="92" t="s">
+      <c r="G7" s="48" t="s">
         <v>123</v>
       </c>
-      <c r="H7" s="92" t="s">
+      <c r="H7" s="48" t="s">
         <v>127</v>
       </c>
-      <c r="I7" s="92"/>
-      <c r="J7" s="92" t="s">
+      <c r="I7" s="48"/>
+      <c r="J7" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="K7" s="92"/>
-      <c r="L7" s="92" t="s">
+      <c r="K7" s="48"/>
+      <c r="L7" s="48" t="s">
         <v>43</v>
       </c>
       <c r="M7" s="28" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="100"/>
-      <c r="B8" s="101"/>
-      <c r="C8" s="101"/>
-      <c r="D8" s="101"/>
-      <c r="E8" s="101"/>
-      <c r="F8" s="101"/>
-      <c r="G8" s="101"/>
-      <c r="H8" s="101"/>
-      <c r="I8" s="101"/>
-      <c r="J8" s="101"/>
-      <c r="K8" s="101"/>
-      <c r="L8" s="101"/>
+    <row r="8" spans="1:14" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="52"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="49"/>
+      <c r="K8" s="49"/>
+      <c r="L8" s="49"/>
       <c r="M8" s="28" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="99"/>
-      <c r="B9" s="93"/>
-      <c r="C9" s="93"/>
-      <c r="D9" s="93"/>
-      <c r="E9" s="93"/>
-      <c r="F9" s="93"/>
-      <c r="G9" s="93"/>
-      <c r="H9" s="93"/>
-      <c r="I9" s="93"/>
-      <c r="J9" s="93"/>
-      <c r="K9" s="93"/>
-      <c r="L9" s="93"/>
+    <row r="9" spans="1:14" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="53"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="50"/>
+      <c r="G9" s="50"/>
+      <c r="H9" s="50"/>
+      <c r="I9" s="50"/>
+      <c r="J9" s="50"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="50"/>
       <c r="M9" s="28" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="27" t="s">
         <v>31</v>
       </c>
@@ -3424,63 +3420,63 @@
         <v>132</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="92" t="s">
+      <c r="B11" s="48" t="s">
         <v>128</v>
       </c>
-      <c r="C11" s="92" t="s">
+      <c r="C11" s="48" t="s">
         <v>129</v>
       </c>
-      <c r="D11" s="92" t="s">
+      <c r="D11" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="92" t="s">
+      <c r="E11" s="48" t="s">
         <v>121</v>
       </c>
-      <c r="F11" s="92" t="s">
+      <c r="F11" s="48" t="s">
         <v>131</v>
       </c>
-      <c r="G11" s="92" t="s">
+      <c r="G11" s="48" t="s">
         <v>123</v>
       </c>
-      <c r="H11" s="92" t="s">
+      <c r="H11" s="48" t="s">
         <v>127</v>
       </c>
-      <c r="I11" s="92"/>
-      <c r="J11" s="92" t="s">
+      <c r="I11" s="48"/>
+      <c r="J11" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="K11" s="92"/>
-      <c r="L11" s="92" t="s">
+      <c r="K11" s="48"/>
+      <c r="L11" s="48" t="s">
         <v>181</v>
       </c>
       <c r="M11" s="28" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="B12" s="93"/>
-      <c r="C12" s="93"/>
-      <c r="D12" s="93"/>
-      <c r="E12" s="93"/>
-      <c r="F12" s="93"/>
-      <c r="G12" s="93"/>
-      <c r="H12" s="93"/>
-      <c r="I12" s="93"/>
-      <c r="J12" s="93"/>
-      <c r="K12" s="93"/>
-      <c r="L12" s="93"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="50"/>
+      <c r="G12" s="50"/>
+      <c r="H12" s="50"/>
+      <c r="I12" s="50"/>
+      <c r="J12" s="50"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="50"/>
       <c r="M12" s="33" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="s">
         <v>31</v>
       </c>
@@ -3517,36 +3513,11 @@
         <v>182</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E14" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="K11:K12"/>
-    <mergeCell ref="L11:L12"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L7:L9"/>
-    <mergeCell ref="K7:K9"/>
-    <mergeCell ref="J7:J9"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="B2:M2"/>
@@ -3562,6 +3533,31 @@
     <mergeCell ref="L4:L6"/>
     <mergeCell ref="M4:M6"/>
     <mergeCell ref="E5:F5"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="K11:K12"/>
+    <mergeCell ref="L11:L12"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L7:L9"/>
+    <mergeCell ref="K7:K9"/>
+    <mergeCell ref="J7:J9"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="B7:B9"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
@@ -3578,111 +3574,111 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{135EFB96-F09D-4669-AFCD-45B4BA78057C}">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView topLeftCell="C9" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="18.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.21875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="28.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="18.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="28.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="38" style="1" customWidth="1"/>
-    <col min="13" max="13" width="46.33203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="132.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="50.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="66.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="52.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.44140625" style="1"/>
+    <col min="13" max="13" width="46.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="132.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="50.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="66.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="52.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="58" t="s">
+      <c r="B2" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="59"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="69"/>
+      <c r="M2" s="70"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="60" t="str">
+      <c r="B3" s="54" t="str">
         <f>'Listado Objetos de Dominio'!$B$7</f>
         <v>Objeto de dominio que representa la Agenda programada de manera especifica para cada zona comun.</v>
       </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="61"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="55"/>
       <c r="N3" s="4"/>
     </row>
-    <row r="4" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="45"/>
+      <c r="C4" s="56"/>
       <c r="D4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="46" t="s">
+      <c r="E4" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="46"/>
-      <c r="G4" s="53" t="s">
+      <c r="F4" s="57"/>
+      <c r="G4" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="53"/>
+      <c r="H4" s="64"/>
       <c r="I4" s="9" t="s">
         <v>14</v>
       </c>
@@ -3692,52 +3688,52 @@
       <c r="K4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="56" t="s">
+      <c r="L4" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="57" t="s">
+      <c r="M4" s="68" t="s">
         <v>18</v>
       </c>
       <c r="N4" s="4"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="50" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="61" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="47" t="s">
+      <c r="D5" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="46"/>
-      <c r="G5" s="51" t="s">
+      <c r="F5" s="57"/>
+      <c r="G5" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="51"/>
-      <c r="I5" s="54" t="s">
+      <c r="H5" s="62"/>
+      <c r="I5" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="55" t="s">
+      <c r="J5" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="52" t="s">
+      <c r="K5" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="56"/>
-      <c r="M5" s="57"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="50"/>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="48"/>
+      <c r="L5" s="67"/>
+      <c r="M5" s="68"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="61"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="59"/>
       <c r="E6" s="11" t="s">
         <v>21</v>
       </c>
@@ -3750,83 +3746,83 @@
       <c r="H6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="54"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="57"/>
-    </row>
-    <row r="7" spans="1:14" ht="94.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="98" t="s">
+      <c r="I6" s="65"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="67"/>
+      <c r="M6" s="68"/>
+    </row>
+    <row r="7" spans="1:14" ht="94.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="51" t="s">
         <v>136</v>
       </c>
-      <c r="B7" s="92" t="s">
+      <c r="B7" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="C7" s="92" t="s">
+      <c r="C7" s="48" t="s">
         <v>61</v>
       </c>
-      <c r="D7" s="92" t="s">
+      <c r="D7" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="92" t="s">
+      <c r="E7" s="48" t="s">
         <v>80</v>
       </c>
-      <c r="F7" s="92" t="s">
+      <c r="F7" s="48" t="s">
         <v>134</v>
       </c>
-      <c r="G7" s="92" t="s">
+      <c r="G7" s="48" t="s">
         <v>73</v>
       </c>
-      <c r="H7" s="92" t="s">
+      <c r="H7" s="48" t="s">
         <v>169</v>
       </c>
-      <c r="I7" s="92"/>
-      <c r="J7" s="92" t="s">
+      <c r="I7" s="48"/>
+      <c r="J7" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="K7" s="92"/>
-      <c r="L7" s="92" t="s">
+      <c r="K7" s="48"/>
+      <c r="L7" s="48" t="s">
         <v>63</v>
       </c>
       <c r="M7" s="29" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="94.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="99"/>
-      <c r="B8" s="93"/>
-      <c r="C8" s="93"/>
-      <c r="D8" s="93"/>
-      <c r="E8" s="93"/>
-      <c r="F8" s="93"/>
-      <c r="G8" s="93"/>
-      <c r="H8" s="93"/>
-      <c r="I8" s="93"/>
-      <c r="J8" s="93"/>
-      <c r="K8" s="93"/>
-      <c r="L8" s="93"/>
+    <row r="8" spans="1:14" ht="94.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="53"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="50"/>
       <c r="M8" s="29" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="72" x14ac:dyDescent="0.3">
-      <c r="A9" s="98" t="s">
+    <row r="9" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="92" t="s">
+      <c r="B9" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="92" t="s">
+      <c r="C9" s="48" t="s">
         <v>64</v>
       </c>
-      <c r="D9" s="92" t="s">
+      <c r="D9" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="92" t="s">
+      <c r="E9" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="F9" s="92" t="s">
+      <c r="F9" s="48" t="s">
         <v>134</v>
       </c>
       <c r="G9" s="24" t="s">
@@ -3835,75 +3831,75 @@
       <c r="H9" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="I9" s="92"/>
-      <c r="J9" s="92" t="s">
+      <c r="I9" s="48"/>
+      <c r="J9" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="K9" s="92"/>
+      <c r="K9" s="48"/>
       <c r="L9" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="M9" s="96" t="s">
+      <c r="M9" s="110" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="100"/>
-      <c r="B10" s="101"/>
-      <c r="C10" s="101"/>
-      <c r="D10" s="101"/>
-      <c r="E10" s="101"/>
-      <c r="F10" s="101"/>
+    <row r="10" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="52"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
       <c r="G10" s="22" t="s">
         <v>73</v>
       </c>
       <c r="H10" s="22" t="s">
         <v>169</v>
       </c>
-      <c r="I10" s="101"/>
-      <c r="J10" s="101"/>
-      <c r="K10" s="101"/>
-      <c r="L10" s="101" t="s">
+      <c r="I10" s="49"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="49"/>
+      <c r="L10" s="49" t="s">
         <v>171</v>
       </c>
-      <c r="M10" s="102"/>
-    </row>
-    <row r="11" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="99"/>
-      <c r="B11" s="93"/>
-      <c r="C11" s="93"/>
-      <c r="D11" s="93"/>
-      <c r="E11" s="93"/>
-      <c r="F11" s="93"/>
+      <c r="M10" s="111"/>
+    </row>
+    <row r="11" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="53"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
       <c r="G11" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="H11" s="109" t="s">
+      <c r="H11" s="39" t="s">
         <v>163</v>
       </c>
-      <c r="I11" s="93"/>
-      <c r="J11" s="93"/>
-      <c r="K11" s="93"/>
-      <c r="L11" s="93"/>
-      <c r="M11" s="97"/>
-    </row>
-    <row r="12" spans="1:14" ht="72" x14ac:dyDescent="0.3">
-      <c r="A12" s="98" t="s">
+      <c r="I11" s="50"/>
+      <c r="J11" s="50"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="50"/>
+      <c r="M11" s="112"/>
+    </row>
+    <row r="12" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+      <c r="A12" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="92" t="s">
+      <c r="B12" s="48" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="92" t="s">
+      <c r="C12" s="48" t="s">
         <v>70</v>
       </c>
-      <c r="D12" s="92" t="s">
+      <c r="D12" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="92" t="s">
+      <c r="E12" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="92" t="s">
+      <c r="F12" s="48" t="s">
         <v>79</v>
       </c>
       <c r="G12" s="24" t="s">
@@ -3912,61 +3908,61 @@
       <c r="H12" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="I12" s="92"/>
-      <c r="J12" s="92" t="s">
+      <c r="I12" s="48"/>
+      <c r="J12" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="K12" s="92"/>
-      <c r="L12" s="92" t="s">
+      <c r="K12" s="48"/>
+      <c r="L12" s="48" t="s">
         <v>45</v>
       </c>
       <c r="M12" s="28" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="100"/>
-      <c r="B13" s="101"/>
-      <c r="C13" s="101"/>
-      <c r="D13" s="101"/>
-      <c r="E13" s="101"/>
-      <c r="F13" s="101"/>
+    <row r="13" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="52"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
       <c r="G13" s="22" t="s">
         <v>73</v>
       </c>
       <c r="H13" s="24" t="s">
         <v>169</v>
       </c>
-      <c r="I13" s="101"/>
-      <c r="J13" s="101"/>
-      <c r="K13" s="101"/>
-      <c r="L13" s="101"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="49"/>
+      <c r="L13" s="49"/>
       <c r="M13" s="28" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="99"/>
-      <c r="B14" s="93"/>
-      <c r="C14" s="93"/>
-      <c r="D14" s="93"/>
-      <c r="E14" s="93"/>
-      <c r="F14" s="93"/>
+    <row r="14" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="53"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
       <c r="G14" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="H14" s="109" t="s">
+      <c r="H14" s="39" t="s">
         <v>163</v>
       </c>
-      <c r="I14" s="93"/>
-      <c r="J14" s="93"/>
-      <c r="K14" s="93"/>
-      <c r="L14" s="93"/>
+      <c r="I14" s="50"/>
+      <c r="J14" s="50"/>
+      <c r="K14" s="50"/>
+      <c r="L14" s="50"/>
       <c r="M14" s="33" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="27" t="s">
         <v>31</v>
       </c>
@@ -4001,36 +3997,6 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="L7:L8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="K12:K14"/>
-    <mergeCell ref="L12:L14"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="K9:K11"/>
-    <mergeCell ref="M9:M11"/>
-    <mergeCell ref="I9:I11"/>
-    <mergeCell ref="F9:F11"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="F12:F14"/>
-    <mergeCell ref="E12:E14"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="D12:D14"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="B12:B14"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="J12:J14"/>
     <mergeCell ref="I12:I14"/>
@@ -4047,10 +4013,40 @@
     <mergeCell ref="B5:B6"/>
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="C5:C6"/>
+    <mergeCell ref="E12:E14"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="D12:D14"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="B12:B14"/>
     <mergeCell ref="D5:D6"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="I5:I6"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="K9:K11"/>
+    <mergeCell ref="M9:M11"/>
+    <mergeCell ref="I9:I11"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="K12:K14"/>
+    <mergeCell ref="L12:L14"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="F12:F14"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="L7:L8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="H7:H8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{175DFE60-DD9E-49DC-B6DD-E705858EF325}"/>
@@ -4065,112 +4061,112 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8BE5EAF-3DFC-48B5-92F6-DF96C5003B3E}">
   <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="69" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="18.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="28.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="18.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="28.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="38" style="1" customWidth="1"/>
-    <col min="13" max="13" width="46.33203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="132.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="50.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="66.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="52.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.44140625" style="1"/>
+    <col min="13" max="13" width="46.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="132.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="50.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="66.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="52.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="58" t="str">
+      <c r="B2" s="69" t="str">
         <f>'Listado Objetos de Dominio'!A9</f>
         <v>Publicación</v>
       </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="59"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="69"/>
+      <c r="M2" s="70"/>
       <c r="N2" s="3"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="60" t="str">
+      <c r="B3" s="54" t="str">
         <f>'Listado Objetos de Dominio'!$B$9</f>
         <v xml:space="preserve"> Objeto de dominio que representa el medio de comunicación que hay frente de publicar alguna eventualidad.</v>
       </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="61"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="55"/>
       <c r="N3" s="4"/>
     </row>
-    <row r="4" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="45" t="s">
+      <c r="B4" s="56" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="45"/>
+      <c r="C4" s="56"/>
       <c r="D4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="46" t="s">
+      <c r="E4" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="46"/>
-      <c r="G4" s="53" t="s">
+      <c r="F4" s="57"/>
+      <c r="G4" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="53"/>
+      <c r="H4" s="64"/>
       <c r="I4" s="9" t="s">
         <v>14</v>
       </c>
@@ -4180,52 +4176,52 @@
       <c r="K4" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="L4" s="56" t="s">
+      <c r="L4" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="57" t="s">
+      <c r="M4" s="68" t="s">
         <v>18</v>
       </c>
       <c r="N4" s="4"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="50" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="47" t="s">
+      <c r="D5" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="46"/>
-      <c r="G5" s="51" t="s">
+      <c r="F5" s="57"/>
+      <c r="G5" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="51"/>
-      <c r="I5" s="54" t="s">
+      <c r="H5" s="62"/>
+      <c r="I5" s="65" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="55" t="s">
+      <c r="J5" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="K5" s="52" t="s">
+      <c r="K5" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="56"/>
-      <c r="M5" s="57"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="50"/>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="48"/>
+      <c r="L5" s="67"/>
+      <c r="M5" s="68"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="61"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="59"/>
       <c r="E6" s="11" t="s">
         <v>21</v>
       </c>
@@ -4238,121 +4234,121 @@
       <c r="H6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="I6" s="54"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="57"/>
-    </row>
-    <row r="7" spans="1:14" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="98" t="s">
+      <c r="I6" s="65"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="67"/>
+      <c r="M6" s="68"/>
+    </row>
+    <row r="7" spans="1:14" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="92" t="s">
+      <c r="B7" s="48" t="s">
         <v>137</v>
       </c>
-      <c r="C7" s="92" t="s">
+      <c r="C7" s="48" t="s">
         <v>138</v>
       </c>
-      <c r="D7" s="92" t="s">
+      <c r="D7" s="48" t="s">
         <v>140</v>
       </c>
-      <c r="E7" s="92" t="s">
+      <c r="E7" s="48" t="s">
         <v>121</v>
       </c>
-      <c r="F7" s="92" t="s">
+      <c r="F7" s="48" t="s">
         <v>141</v>
       </c>
-      <c r="G7" s="92" t="s">
+      <c r="G7" s="48" t="s">
         <v>142</v>
       </c>
-      <c r="H7" s="92" t="s">
+      <c r="H7" s="48" t="s">
         <v>143</v>
       </c>
-      <c r="I7" s="92"/>
-      <c r="J7" s="92" t="s">
+      <c r="I7" s="48"/>
+      <c r="J7" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="K7" s="92"/>
-      <c r="L7" s="92" t="s">
+      <c r="K7" s="48"/>
+      <c r="L7" s="48" t="s">
         <v>183</v>
       </c>
       <c r="M7" s="28" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="100"/>
-      <c r="B8" s="101"/>
-      <c r="C8" s="101"/>
-      <c r="D8" s="101"/>
-      <c r="E8" s="101"/>
-      <c r="F8" s="101"/>
-      <c r="G8" s="93"/>
-      <c r="H8" s="93"/>
-      <c r="I8" s="101"/>
-      <c r="J8" s="101"/>
-      <c r="K8" s="101"/>
-      <c r="L8" s="101"/>
+    <row r="8" spans="1:14" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="52"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="49"/>
+      <c r="K8" s="49"/>
+      <c r="L8" s="49"/>
       <c r="M8" s="33" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="100"/>
-      <c r="B9" s="101"/>
-      <c r="C9" s="101"/>
-      <c r="D9" s="101"/>
-      <c r="E9" s="101"/>
-      <c r="F9" s="101"/>
-      <c r="G9" s="92" t="s">
+    <row r="9" spans="1:14" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="52"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="48" t="s">
         <v>144</v>
       </c>
-      <c r="H9" s="92" t="s">
+      <c r="H9" s="48" t="s">
         <v>145</v>
       </c>
-      <c r="I9" s="101"/>
-      <c r="J9" s="101"/>
-      <c r="K9" s="101"/>
-      <c r="L9" s="101"/>
+      <c r="I9" s="49"/>
+      <c r="J9" s="49"/>
+      <c r="K9" s="49"/>
+      <c r="L9" s="49"/>
       <c r="M9" s="28" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="99"/>
-      <c r="B10" s="93"/>
-      <c r="C10" s="93"/>
-      <c r="D10" s="93"/>
-      <c r="E10" s="93"/>
-      <c r="F10" s="93"/>
-      <c r="G10" s="93"/>
-      <c r="H10" s="93"/>
-      <c r="I10" s="93"/>
-      <c r="J10" s="93"/>
-      <c r="K10" s="93"/>
-      <c r="L10" s="93"/>
+    <row r="10" spans="1:14" ht="39.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="53"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="50"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="50"/>
       <c r="M10" s="35" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="78.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="34" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="92" t="s">
+      <c r="B11" s="48" t="s">
         <v>146</v>
       </c>
-      <c r="C11" s="92" t="s">
+      <c r="C11" s="48" t="s">
         <v>147</v>
       </c>
-      <c r="D11" s="92" t="s">
+      <c r="D11" s="48" t="s">
         <v>140</v>
       </c>
-      <c r="E11" s="92" t="s">
+      <c r="E11" s="48" t="s">
         <v>121</v>
       </c>
-      <c r="F11" s="92" t="s">
+      <c r="F11" s="48" t="s">
         <v>150</v>
       </c>
       <c r="G11" s="24" t="s">
@@ -4361,75 +4357,75 @@
       <c r="H11" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="I11" s="92"/>
-      <c r="J11" s="92" t="s">
+      <c r="I11" s="48"/>
+      <c r="J11" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="K11" s="92"/>
-      <c r="L11" s="92" t="s">
+      <c r="K11" s="48"/>
+      <c r="L11" s="48" t="s">
         <v>186</v>
       </c>
       <c r="M11" s="28" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="98" t="s">
+    <row r="12" spans="1:14" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="B12" s="101"/>
-      <c r="C12" s="101"/>
-      <c r="D12" s="101"/>
-      <c r="E12" s="101"/>
-      <c r="F12" s="101"/>
-      <c r="G12" s="92" t="s">
+      <c r="B12" s="49"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="48" t="s">
         <v>144</v>
       </c>
-      <c r="H12" s="92" t="s">
+      <c r="H12" s="48" t="s">
         <v>145</v>
       </c>
-      <c r="I12" s="101"/>
-      <c r="J12" s="101"/>
-      <c r="K12" s="101"/>
-      <c r="L12" s="101"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="49"/>
+      <c r="K12" s="49"/>
+      <c r="L12" s="49"/>
       <c r="M12" s="33" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="99"/>
-      <c r="B13" s="93"/>
-      <c r="C13" s="93"/>
-      <c r="D13" s="93"/>
-      <c r="E13" s="93"/>
-      <c r="F13" s="93"/>
-      <c r="G13" s="93"/>
-      <c r="H13" s="93"/>
-      <c r="I13" s="93"/>
-      <c r="J13" s="93"/>
-      <c r="K13" s="93"/>
-      <c r="L13" s="93"/>
+    <row r="13" spans="1:14" ht="37.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="53"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50"/>
+      <c r="G13" s="50"/>
+      <c r="H13" s="50"/>
+      <c r="I13" s="50"/>
+      <c r="J13" s="50"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="50"/>
       <c r="M13" s="35" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="70.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="98" t="s">
+    <row r="14" spans="1:14" ht="70.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="92" t="s">
+      <c r="B14" s="48" t="s">
         <v>148</v>
       </c>
-      <c r="C14" s="92" t="s">
+      <c r="C14" s="48" t="s">
         <v>149</v>
       </c>
-      <c r="D14" s="92" t="s">
+      <c r="D14" s="48" t="s">
         <v>140</v>
       </c>
-      <c r="E14" s="92" t="s">
+      <c r="E14" s="48" t="s">
         <v>121</v>
       </c>
-      <c r="F14" s="92" t="s">
+      <c r="F14" s="48" t="s">
         <v>154</v>
       </c>
       <c r="G14" s="24" t="s">
@@ -4438,40 +4434,40 @@
       <c r="H14" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="I14" s="92"/>
-      <c r="J14" s="92" t="s">
+      <c r="I14" s="48"/>
+      <c r="J14" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="K14" s="92"/>
-      <c r="L14" s="92" t="s">
+      <c r="K14" s="48"/>
+      <c r="L14" s="48" t="s">
         <v>46</v>
       </c>
       <c r="M14" s="29" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="70.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="99"/>
-      <c r="B15" s="93"/>
-      <c r="C15" s="93"/>
-      <c r="D15" s="93"/>
-      <c r="E15" s="93"/>
-      <c r="F15" s="93"/>
+    <row r="15" spans="1:14" ht="70.900000000000006" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="53"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
       <c r="G15" s="24" t="s">
         <v>144</v>
       </c>
       <c r="H15" s="24" t="s">
         <v>145</v>
       </c>
-      <c r="I15" s="93"/>
-      <c r="J15" s="93"/>
-      <c r="K15" s="93"/>
-      <c r="L15" s="93"/>
+      <c r="I15" s="50"/>
+      <c r="J15" s="50"/>
+      <c r="K15" s="50"/>
+      <c r="L15" s="50"/>
       <c r="M15" s="33" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="72" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
         <v>31</v>
       </c>
@@ -4504,23 +4500,23 @@
         <v>187</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="72" x14ac:dyDescent="0.3">
-      <c r="A17" s="98" t="s">
+    <row r="17" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="51" t="s">
         <v>90</v>
       </c>
-      <c r="B17" s="92" t="s">
+      <c r="B17" s="48" t="s">
         <v>155</v>
       </c>
-      <c r="C17" s="92" t="s">
+      <c r="C17" s="48" t="s">
         <v>156</v>
       </c>
-      <c r="D17" s="92" t="s">
+      <c r="D17" s="48" t="s">
         <v>140</v>
       </c>
-      <c r="E17" s="92" t="s">
+      <c r="E17" s="48" t="s">
         <v>121</v>
       </c>
-      <c r="F17" s="92" t="s">
+      <c r="F17" s="48" t="s">
         <v>153</v>
       </c>
       <c r="G17" s="24" t="s">
@@ -4529,59 +4525,70 @@
       <c r="H17" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="I17" s="92"/>
-      <c r="J17" s="92" t="s">
+      <c r="I17" s="48"/>
+      <c r="J17" s="48" t="s">
         <v>50</v>
       </c>
-      <c r="K17" s="92"/>
-      <c r="L17" s="92" t="s">
+      <c r="K17" s="48"/>
+      <c r="L17" s="48" t="s">
         <v>46</v>
       </c>
       <c r="M17" s="28" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="99"/>
-      <c r="B18" s="93"/>
-      <c r="C18" s="93"/>
-      <c r="D18" s="93"/>
-      <c r="E18" s="93"/>
-      <c r="F18" s="93"/>
+    <row r="18" spans="1:13" ht="59.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="53"/>
+      <c r="B18" s="50"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
       <c r="G18" s="24" t="s">
         <v>144</v>
       </c>
       <c r="H18" s="24" t="s">
         <v>145</v>
       </c>
-      <c r="I18" s="93"/>
-      <c r="J18" s="93"/>
-      <c r="K18" s="93"/>
-      <c r="L18" s="93"/>
+      <c r="I18" s="50"/>
+      <c r="J18" s="50"/>
+      <c r="K18" s="50"/>
+      <c r="L18" s="50"/>
       <c r="M18" s="33" t="s">
         <v>185</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="J11:J13"/>
-    <mergeCell ref="I11:I13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="L17:L18"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="L7:L10"/>
-    <mergeCell ref="K7:K10"/>
-    <mergeCell ref="L11:L13"/>
-    <mergeCell ref="K11:K13"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B3:M3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="L4:L6"/>
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="B7:B10"/>
+    <mergeCell ref="A7:A10"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="F7:F10"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E7:E10"/>
+    <mergeCell ref="D7:D10"/>
+    <mergeCell ref="C7:C10"/>
+    <mergeCell ref="J7:J10"/>
+    <mergeCell ref="I7:I10"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="J14:J15"/>
     <mergeCell ref="A17:A18"/>
@@ -4598,21 +4605,419 @@
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="B14:B15"/>
-    <mergeCell ref="J7:J10"/>
-    <mergeCell ref="I7:I10"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="F7:F10"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E7:E10"/>
-    <mergeCell ref="D7:D10"/>
-    <mergeCell ref="C7:C10"/>
-    <mergeCell ref="B7:B10"/>
-    <mergeCell ref="A7:A10"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="L7:L10"/>
+    <mergeCell ref="K7:K10"/>
+    <mergeCell ref="L11:L13"/>
+    <mergeCell ref="K11:K13"/>
+    <mergeCell ref="J11:J13"/>
+    <mergeCell ref="I11:I13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="A12:A13"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{755244C2-D34A-4436-ABEF-3130787CFBF9}"/>
+    <hyperlink ref="A1:N1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{F5A9893C-CE5B-47AC-8BA0-456E89214E9A}"/>
+    <hyperlink ref="D1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{238F79C9-7DA8-4F58-84A3-6CBEF6586270}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC47FB83-9179-46D6-840D-CDDDAC34ECFB}">
+  <dimension ref="A1:N20"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="18.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="34.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="38" style="1" customWidth="1"/>
+    <col min="13" max="13" width="46.28515625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="19.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="132.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="46.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="50.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="66.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="52.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="60"/>
+      <c r="J1" s="60"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="60"/>
+      <c r="M1" s="60"/>
+      <c r="N1" s="60"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="69" t="str">
+        <f>'Listado Objetos de Dominio'!A8</f>
+        <v>Turno</v>
+      </c>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="69"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="3"/>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="54" t="str">
+        <f>'Listado Objetos de Dominio'!$B$8</f>
+        <v>Objeto de dominio que representa a cada Turno que esta programado con respecto al tiempo de uso según la zona comun y con respecto a la agenda disponible.</v>
+      </c>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="55"/>
+      <c r="N3" s="4"/>
+    </row>
+    <row r="4" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="56" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="56"/>
+      <c r="D4" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="57" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="57"/>
+      <c r="G4" s="64" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="64"/>
+      <c r="I4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="67" t="s">
+        <v>17</v>
+      </c>
+      <c r="M4" s="68" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" s="4"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="61" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="56" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="56" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="58" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="57" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="57"/>
+      <c r="G5" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="62"/>
+      <c r="I5" s="65" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" s="66" t="s">
+        <v>8</v>
+      </c>
+      <c r="K5" s="63" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="67"/>
+      <c r="M5" s="68"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="61"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" s="65"/>
+      <c r="J6" s="66"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="67"/>
+      <c r="M6" s="68"/>
+    </row>
+    <row r="7" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A7" s="77" t="s">
+        <v>136</v>
+      </c>
+      <c r="B7" s="77" t="s">
+        <v>188</v>
+      </c>
+      <c r="C7" s="77" t="s">
+        <v>189</v>
+      </c>
+      <c r="D7" s="77" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="77" t="s">
+        <v>190</v>
+      </c>
+      <c r="F7" s="77" t="s">
+        <v>191</v>
+      </c>
+      <c r="G7" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="H7" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="I7" s="77"/>
+      <c r="J7" s="77" t="s">
+        <v>51</v>
+      </c>
+      <c r="K7" s="77"/>
+      <c r="L7" s="77" t="s">
+        <v>52</v>
+      </c>
+      <c r="M7" s="24" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="153" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="77"/>
+      <c r="B8" s="77"/>
+      <c r="C8" s="77"/>
+      <c r="D8" s="77"/>
+      <c r="E8" s="77"/>
+      <c r="F8" s="77"/>
+      <c r="G8" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="H8" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="I8" s="77"/>
+      <c r="J8" s="77"/>
+      <c r="K8" s="77"/>
+      <c r="L8" s="77"/>
+      <c r="M8" s="77" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="77"/>
+      <c r="B9" s="77"/>
+      <c r="C9" s="77"/>
+      <c r="D9" s="77"/>
+      <c r="E9" s="77"/>
+      <c r="F9" s="77"/>
+      <c r="G9" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="H9" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="I9" s="77"/>
+      <c r="J9" s="77"/>
+      <c r="K9" s="77"/>
+      <c r="L9" s="77"/>
+      <c r="M9" s="77"/>
+    </row>
+    <row r="10" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" s="77" t="s">
+        <v>136</v>
+      </c>
+      <c r="B10" s="77" t="s">
+        <v>192</v>
+      </c>
+      <c r="C10" s="77" t="s">
+        <v>193</v>
+      </c>
+      <c r="D10" s="77" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="77" t="s">
+        <v>190</v>
+      </c>
+      <c r="F10" s="77" t="s">
+        <v>191</v>
+      </c>
+      <c r="G10" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="H10" s="24" t="s">
+        <v>166</v>
+      </c>
+      <c r="I10" s="77"/>
+      <c r="J10" s="77" t="s">
+        <v>76</v>
+      </c>
+      <c r="K10" s="74"/>
+      <c r="L10" s="77" t="s">
+        <v>51</v>
+      </c>
+      <c r="M10" s="77" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="142.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="77"/>
+      <c r="B11" s="77"/>
+      <c r="C11" s="77"/>
+      <c r="D11" s="77"/>
+      <c r="E11" s="77"/>
+      <c r="F11" s="77"/>
+      <c r="G11" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="H11" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="I11" s="77"/>
+      <c r="J11" s="77"/>
+      <c r="K11" s="76"/>
+      <c r="L11" s="77"/>
+      <c r="M11" s="77"/>
+    </row>
+    <row r="12" spans="1:14" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="77"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="77"/>
+      <c r="D12" s="77"/>
+      <c r="E12" s="77"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="H12" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="I12" s="77"/>
+      <c r="J12" s="77"/>
+      <c r="K12" s="75"/>
+      <c r="L12" s="77"/>
+      <c r="M12" s="77"/>
+    </row>
+    <row r="13" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>191</v>
+      </c>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="K13" s="24"/>
+      <c r="L13" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="M13" s="24" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H16" s="36"/>
+    </row>
+    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H17" s="36"/>
+    </row>
+    <row r="18" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H18" s="36"/>
+    </row>
+    <row r="19" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H19" s="36"/>
+    </row>
+    <row r="20" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H20" s="36"/>
+    </row>
+  </sheetData>
+  <mergeCells count="39">
     <mergeCell ref="J5:J6"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="B2:M2"/>
@@ -4627,401 +5032,15 @@
     <mergeCell ref="K5:K6"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="D5:D6"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{755244C2-D34A-4436-ABEF-3130787CFBF9}"/>
-    <hyperlink ref="A1:N1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{F5A9893C-CE5B-47AC-8BA0-456E89214E9A}"/>
-    <hyperlink ref="D1" location="'Listado Objetos de Dominio'!A1" display="&lt;-Volver al inicio" xr:uid="{238F79C9-7DA8-4F58-84A3-6CBEF6586270}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC47FB83-9179-46D6-840D-CDDDAC34ECFB}">
-  <dimension ref="A1:N20"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.44140625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="18.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.44140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="34.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="38" style="1" customWidth="1"/>
-    <col min="13" max="13" width="46.33203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="132.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="46.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="50.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="66.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="52.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="11.44140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="49" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="58" t="str">
-        <f>'Listado Objetos de Dominio'!A8</f>
-        <v>Turno</v>
-      </c>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="58"/>
-      <c r="J2" s="58"/>
-      <c r="K2" s="58"/>
-      <c r="L2" s="58"/>
-      <c r="M2" s="59"/>
-      <c r="N2" s="3"/>
-    </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="60" t="str">
-        <f>'Listado Objetos de Dominio'!$B$8</f>
-        <v>Objeto de dominio que representa a cada Turno que esta programado con respecto al tiempo de uso según la zona comun y con respecto a la agenda disponible.</v>
-      </c>
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="61"/>
-      <c r="N3" s="4"/>
-    </row>
-    <row r="4" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="45" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="45"/>
-      <c r="D4" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="46" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="46"/>
-      <c r="G4" s="53" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="53"/>
-      <c r="I4" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="L4" s="56" t="s">
-        <v>17</v>
-      </c>
-      <c r="M4" s="57" t="s">
-        <v>18</v>
-      </c>
-      <c r="N4" s="4"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="50" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="45" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="47" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="46"/>
-      <c r="G5" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="H5" s="51"/>
-      <c r="I5" s="54" t="s">
-        <v>15</v>
-      </c>
-      <c r="J5" s="55" t="s">
-        <v>8</v>
-      </c>
-      <c r="K5" s="52" t="s">
-        <v>10</v>
-      </c>
-      <c r="L5" s="56"/>
-      <c r="M5" s="57"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="50"/>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="I6" s="54"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="52"/>
-      <c r="L6" s="56"/>
-      <c r="M6" s="57"/>
-    </row>
-    <row r="7" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="110" t="s">
-        <v>136</v>
-      </c>
-      <c r="B7" s="110" t="s">
-        <v>188</v>
-      </c>
-      <c r="C7" s="110" t="s">
-        <v>189</v>
-      </c>
-      <c r="D7" s="110" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="110" t="s">
-        <v>190</v>
-      </c>
-      <c r="F7" s="110" t="s">
-        <v>191</v>
-      </c>
-      <c r="G7" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="H7" s="24" t="s">
-        <v>166</v>
-      </c>
-      <c r="I7" s="110"/>
-      <c r="J7" s="110" t="s">
-        <v>51</v>
-      </c>
-      <c r="K7" s="110"/>
-      <c r="L7" s="110" t="s">
-        <v>52</v>
-      </c>
-      <c r="M7" s="24" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="153" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="110"/>
-      <c r="B8" s="110"/>
-      <c r="C8" s="110"/>
-      <c r="D8" s="110"/>
-      <c r="E8" s="110"/>
-      <c r="F8" s="110"/>
-      <c r="G8" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="H8" s="24" t="s">
-        <v>165</v>
-      </c>
-      <c r="I8" s="110"/>
-      <c r="J8" s="110"/>
-      <c r="K8" s="110"/>
-      <c r="L8" s="110"/>
-      <c r="M8" s="110" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="110"/>
-      <c r="B9" s="110"/>
-      <c r="C9" s="110"/>
-      <c r="D9" s="110"/>
-      <c r="E9" s="110"/>
-      <c r="F9" s="110"/>
-      <c r="G9" s="23" t="s">
-        <v>167</v>
-      </c>
-      <c r="H9" s="24" t="s">
-        <v>166</v>
-      </c>
-      <c r="I9" s="110"/>
-      <c r="J9" s="110"/>
-      <c r="K9" s="110"/>
-      <c r="L9" s="110"/>
-      <c r="M9" s="110"/>
-    </row>
-    <row r="10" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="110" t="s">
-        <v>136</v>
-      </c>
-      <c r="B10" s="110" t="s">
-        <v>192</v>
-      </c>
-      <c r="C10" s="110" t="s">
-        <v>193</v>
-      </c>
-      <c r="D10" s="110" t="s">
-        <v>33</v>
-      </c>
-      <c r="E10" s="110" t="s">
-        <v>190</v>
-      </c>
-      <c r="F10" s="110" t="s">
-        <v>191</v>
-      </c>
-      <c r="G10" s="23" t="s">
-        <v>77</v>
-      </c>
-      <c r="H10" s="24" t="s">
-        <v>166</v>
-      </c>
-      <c r="I10" s="110"/>
-      <c r="J10" s="110" t="s">
-        <v>76</v>
-      </c>
-      <c r="K10" s="94"/>
-      <c r="L10" s="110" t="s">
-        <v>51</v>
-      </c>
-      <c r="M10" s="110" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="142.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="110"/>
-      <c r="B11" s="110"/>
-      <c r="C11" s="110"/>
-      <c r="D11" s="110"/>
-      <c r="E11" s="110"/>
-      <c r="F11" s="110"/>
-      <c r="G11" s="23" t="s">
-        <v>164</v>
-      </c>
-      <c r="H11" s="24" t="s">
-        <v>165</v>
-      </c>
-      <c r="I11" s="110"/>
-      <c r="J11" s="110"/>
-      <c r="K11" s="105"/>
-      <c r="L11" s="110"/>
-      <c r="M11" s="110"/>
-    </row>
-    <row r="12" spans="1:14" ht="84" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="110"/>
-      <c r="B12" s="110"/>
-      <c r="C12" s="110"/>
-      <c r="D12" s="110"/>
-      <c r="E12" s="110"/>
-      <c r="F12" s="110"/>
-      <c r="G12" s="23" t="s">
-        <v>167</v>
-      </c>
-      <c r="H12" s="24" t="s">
-        <v>168</v>
-      </c>
-      <c r="I12" s="110"/>
-      <c r="J12" s="110"/>
-      <c r="K12" s="95"/>
-      <c r="L12" s="110"/>
-      <c r="M12" s="110"/>
-    </row>
-    <row r="13" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="24" t="s">
-        <v>136</v>
-      </c>
-      <c r="B13" s="24" t="s">
-        <v>194</v>
-      </c>
-      <c r="C13" s="24" t="s">
-        <v>195</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" s="24" t="s">
-        <v>190</v>
-      </c>
-      <c r="F13" s="24" t="s">
-        <v>191</v>
-      </c>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="K13" s="24"/>
-      <c r="L13" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="M13" s="24" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="H16" s="36"/>
-    </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H17" s="36"/>
-    </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H18" s="36"/>
-    </row>
-    <row r="19" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H19" s="36"/>
-    </row>
-    <row r="20" spans="8:8" x14ac:dyDescent="0.3">
-      <c r="H20" s="36"/>
-    </row>
-  </sheetData>
-  <mergeCells count="39">
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="L7:L9"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E9"/>
     <mergeCell ref="M8:M9"/>
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="B10:B12"/>
@@ -5038,29 +5057,6 @@
     <mergeCell ref="I7:I9"/>
     <mergeCell ref="J7:J9"/>
     <mergeCell ref="K7:K9"/>
-    <mergeCell ref="L7:L9"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="B3:M3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="L4:L6"/>
-    <mergeCell ref="M4:M6"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1" location="'Objetos de Dominio'!A1" display="Volver al inicio" xr:uid="{72BB53BB-A255-4E65-8E13-6A32013B466E}"/>
@@ -5072,12 +5068,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5225,15 +5218,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6724C681-8A04-4D66-BB1C-57F7466573C0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2038022-656B-4A1B-A485-51A1972238BD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="ff57c5a0-3efd-4333-8513-2b909ca014ae"/>
+    <ds:schemaRef ds:uri="0d2457a1-fe8a-4cb2-a5c3-c59e87d2493e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5257,18 +5262,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2038022-656B-4A1B-A485-51A1972238BD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6724C681-8A04-4D66-BB1C-57F7466573C0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="ff57c5a0-3efd-4333-8513-2b909ca014ae"/>
-    <ds:schemaRef ds:uri="0d2457a1-fe8a-4cb2-a5c3-c59e87d2493e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>